<commit_message>
something started to work
</commit_message>
<xml_diff>
--- a/data/Lyme Disease Research-1-4.xlsx
+++ b/data/Lyme Disease Research-1-4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NW460\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NW460\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3920C2C9-5435-49DB-9B13-368148705C5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87913348-6997-4D50-AEA4-614F9918193D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Combined!$A$1:$Q$273</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$K$11:$K$29</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$L$11:$L$29</definedName>
     <definedName name="solver_adj_ob" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_adj_ob1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_cha" localSheetId="2" hidden="1">0</definedName>
@@ -225,13 +225,13 @@
     <definedName name="solver_lhs27" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs28" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs29" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$K$11:$K$29</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$L$11:$L$29</definedName>
     <definedName name="solver_lhs30" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs31" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs32" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs33" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
     <definedName name="solver_lhs34" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!#REF!</definedName>
-    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$L$11:$L$29</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$W$31</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$W$31</definedName>
     <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$L$11:$L$29</definedName>
     <definedName name="solver_lhs7" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$L$11:$L$29</definedName>
@@ -241,10 +241,10 @@
     <definedName name="solver_mod" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ntr" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ntri" hidden="1">1000</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_obc" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_obp" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$Q$30</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Model - Rough with weights (2)'!$W$31</definedName>
     <definedName name="solver_opt_ob" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_psi" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rdp" localSheetId="2" hidden="1">0</definedName>
@@ -304,13 +304,13 @@
     <definedName name="solver_rel27" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel28" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel29" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel30" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel31" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel32" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel33" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel34" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_rel4" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel7" localSheetId="2" hidden="1">5</definedName>
@@ -318,7 +318,7 @@
     <definedName name="solver_rel9" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">19500</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">2100</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">-80</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">-80</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsmp" hidden="1">2</definedName>
@@ -351,7 +351,7 @@
     <definedName name="solver_rxc32" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rxc33" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rxc34" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rxc4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rxc4" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rxc5" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rxc6" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rxc7" localSheetId="2" hidden="1">1</definedName>
@@ -376,7 +376,6 @@
     <definedName name="solver_vst" localSheetId="2" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -8146,23 +8145,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8177,6 +8159,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8548,20 +8547,20 @@
       <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="90"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="81" t="s">
         <v>17</v>
       </c>
     </row>
@@ -8578,16 +8577,16 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="91" t="s">
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="91"/>
+      <c r="I2" s="84"/>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="89"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -8598,34 +8597,34 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
       <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="89"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="89"/>
+      <c r="K4" s="82"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
       <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
@@ -8633,7 +8632,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="89"/>
+      <c r="K5" s="82"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -9858,21 +9857,21 @@
       <c r="C44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="85" t="s">
+      <c r="D44" s="88" t="s">
         <v>60</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F44" s="87" t="s">
+      <c r="F44" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G44" s="87"/>
-      <c r="H44" s="87" t="s">
+      <c r="G44" s="90"/>
+      <c r="H44" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="I44" s="87"/>
-      <c r="J44" s="85" t="s">
+      <c r="I44" s="90"/>
+      <c r="J44" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -9883,173 +9882,173 @@
       <c r="C45" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="86"/>
+      <c r="D45" s="89"/>
       <c r="E45" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="84" t="s">
+      <c r="F45" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G45" s="84"/>
-      <c r="H45" s="84" t="s">
+      <c r="G45" s="87"/>
+      <c r="H45" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="I45" s="84"/>
-      <c r="J45" s="86"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="89"/>
     </row>
     <row r="46" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="9"/>
-      <c r="D46" s="86"/>
+      <c r="D46" s="89"/>
       <c r="E46" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="84" t="s">
+      <c r="F46" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84" t="s">
+      <c r="G46" s="87"/>
+      <c r="H46" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="I46" s="84"/>
-      <c r="J46" s="86"/>
+      <c r="I46" s="87"/>
+      <c r="J46" s="89"/>
     </row>
     <row r="47" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
-      <c r="D47" s="86"/>
+      <c r="D47" s="89"/>
       <c r="E47" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="84" t="s">
+      <c r="F47" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84" t="s">
+      <c r="G47" s="87"/>
+      <c r="H47" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="I47" s="84"/>
-      <c r="J47" s="86"/>
+      <c r="I47" s="87"/>
+      <c r="J47" s="89"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
-      <c r="D48" s="86"/>
+      <c r="D48" s="89"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="84" t="s">
+      <c r="F48" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="84"/>
-      <c r="H48" s="84" t="s">
+      <c r="G48" s="87"/>
+      <c r="H48" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="I48" s="84"/>
-      <c r="J48" s="86"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="89"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
-      <c r="D49" s="86"/>
+      <c r="D49" s="89"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="84" t="s">
+      <c r="F49" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="84"/>
-      <c r="H49" s="84" t="s">
+      <c r="G49" s="87"/>
+      <c r="H49" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="I49" s="84"/>
-      <c r="J49" s="86"/>
+      <c r="I49" s="87"/>
+      <c r="J49" s="89"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
-      <c r="D50" s="86"/>
+      <c r="D50" s="89"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="84" t="s">
+      <c r="F50" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="84"/>
-      <c r="H50" s="84" t="s">
+      <c r="G50" s="87"/>
+      <c r="H50" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="I50" s="84"/>
-      <c r="J50" s="86"/>
+      <c r="I50" s="87"/>
+      <c r="J50" s="89"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
-      <c r="D51" s="86"/>
+      <c r="D51" s="89"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="84" t="s">
+      <c r="F51" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="G51" s="84"/>
-      <c r="H51" s="84" t="s">
+      <c r="G51" s="87"/>
+      <c r="H51" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="I51" s="84"/>
-      <c r="J51" s="86"/>
+      <c r="I51" s="87"/>
+      <c r="J51" s="89"/>
     </row>
     <row r="52" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
-      <c r="D52" s="86"/>
+      <c r="D52" s="89"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="84" t="s">
+      <c r="F52" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="G52" s="84"/>
-      <c r="H52" s="84" t="s">
+      <c r="G52" s="87"/>
+      <c r="H52" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="I52" s="84"/>
-      <c r="J52" s="86"/>
+      <c r="I52" s="87"/>
+      <c r="J52" s="89"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
-      <c r="D53" s="86"/>
+      <c r="D53" s="89"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="84" t="s">
+      <c r="F53" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="G53" s="84"/>
-      <c r="H53" s="84" t="s">
+      <c r="G53" s="87"/>
+      <c r="H53" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="I53" s="84"/>
-      <c r="J53" s="86"/>
+      <c r="I53" s="87"/>
+      <c r="J53" s="89"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="81"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="82"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="82"/>
-      <c r="J54" s="81"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="91"/>
+      <c r="D54" s="91"/>
+      <c r="E54" s="91"/>
+      <c r="F54" s="92"/>
+      <c r="G54" s="92"/>
+      <c r="H54" s="92"/>
+      <c r="I54" s="92"/>
+      <c r="J54" s="91"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="81"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="81"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="91"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="93"/>
+      <c r="J55" s="91"/>
     </row>
     <row r="56" spans="1:10" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B56" s="81"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
+      <c r="B56" s="91"/>
+      <c r="C56" s="91"/>
+      <c r="D56" s="91"/>
+      <c r="E56" s="91"/>
       <c r="F56" s="9" t="s">
         <v>73</v>
       </c>
@@ -10062,13 +10061,13 @@
       <c r="I56" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J56" s="81"/>
+      <c r="J56" s="91"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="81"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="91"/>
+      <c r="D57" s="91"/>
+      <c r="E57" s="91"/>
       <c r="F57" s="9" t="s">
         <v>74</v>
       </c>
@@ -10081,7 +10080,7 @@
       <c r="I57" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J57" s="81"/>
+      <c r="J57" s="91"/>
     </row>
     <row r="58" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -10263,7 +10262,7 @@
       <c r="G65" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="H65" s="85" t="s">
+      <c r="H65" s="88" t="s">
         <v>60</v>
       </c>
       <c r="I65" s="13" t="s">
@@ -10272,14 +10271,14 @@
       <c r="J65" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K65" s="87" t="s">
+      <c r="K65" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="L65" s="87"/>
+      <c r="L65" s="90"/>
       <c r="M65" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="N65" s="85" t="s">
+      <c r="N65" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -10302,21 +10301,21 @@
       <c r="G66" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H66" s="86"/>
+      <c r="H66" s="89"/>
       <c r="I66" s="9" t="s">
         <v>119</v>
       </c>
       <c r="J66" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K66" s="84" t="s">
+      <c r="K66" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="L66" s="84"/>
+      <c r="L66" s="87"/>
       <c r="M66" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="N66" s="86"/>
+      <c r="N66" s="89"/>
     </row>
     <row r="67" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B67" s="9" t="s">
@@ -10329,21 +10328,21 @@
       <c r="G67" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H67" s="86"/>
+      <c r="H67" s="89"/>
       <c r="I67" s="9" t="s">
         <v>120</v>
       </c>
       <c r="J67" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K67" s="84" t="s">
+      <c r="K67" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="L67" s="84"/>
+      <c r="L67" s="87"/>
       <c r="M67" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="N67" s="86"/>
+      <c r="N67" s="89"/>
     </row>
     <row r="68" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B68" s="9" t="s">
@@ -10356,21 +10355,21 @@
       <c r="G68" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H68" s="86"/>
+      <c r="H68" s="89"/>
       <c r="I68" s="9" t="s">
         <v>121</v>
       </c>
       <c r="J68" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K68" s="84" t="s">
+      <c r="K68" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="L68" s="84"/>
+      <c r="L68" s="87"/>
       <c r="M68" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="N68" s="86"/>
+      <c r="N68" s="89"/>
     </row>
     <row r="69" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B69" s="9"/>
@@ -10381,17 +10380,17 @@
       <c r="G69" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="H69" s="86"/>
+      <c r="H69" s="89"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
-      <c r="K69" s="84" t="s">
+      <c r="K69" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="L69" s="84"/>
+      <c r="L69" s="87"/>
       <c r="M69" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="N69" s="86"/>
+      <c r="N69" s="89"/>
     </row>
     <row r="70" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B70" s="9"/>
@@ -10400,17 +10399,17 @@
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
-      <c r="H70" s="86"/>
+      <c r="H70" s="89"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
-      <c r="K70" s="84" t="s">
+      <c r="K70" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="L70" s="84"/>
+      <c r="L70" s="87"/>
       <c r="M70" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="N70" s="86"/>
+      <c r="N70" s="89"/>
     </row>
     <row r="71" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B71" s="9"/>
@@ -10419,17 +10418,17 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
-      <c r="H71" s="86"/>
+      <c r="H71" s="89"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
-      <c r="K71" s="84" t="s">
+      <c r="K71" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="L71" s="84"/>
+      <c r="L71" s="87"/>
       <c r="M71" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="N71" s="86"/>
+      <c r="N71" s="89"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B72" s="9"/>
@@ -10438,17 +10437,17 @@
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
-      <c r="H72" s="86"/>
+      <c r="H72" s="89"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
-      <c r="K72" s="84" t="s">
+      <c r="K72" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="L72" s="84"/>
+      <c r="L72" s="87"/>
       <c r="M72" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="N72" s="86"/>
+      <c r="N72" s="89"/>
     </row>
     <row r="73" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="9"/>
@@ -10457,17 +10456,17 @@
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
-      <c r="H73" s="86"/>
+      <c r="H73" s="89"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
-      <c r="K73" s="84" t="s">
+      <c r="K73" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="L73" s="84"/>
+      <c r="L73" s="87"/>
       <c r="M73" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="N73" s="86"/>
+      <c r="N73" s="89"/>
     </row>
     <row r="74" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B74" s="9"/>
@@ -10476,85 +10475,85 @@
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
-      <c r="H74" s="86"/>
+      <c r="H74" s="89"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
-      <c r="K74" s="84" t="s">
+      <c r="K74" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="L74" s="84"/>
+      <c r="L74" s="87"/>
       <c r="M74" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="N74" s="86"/>
+      <c r="N74" s="89"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B75" s="81"/>
-      <c r="C75" s="81"/>
-      <c r="D75" s="81"/>
-      <c r="E75" s="81"/>
-      <c r="F75" s="81"/>
-      <c r="G75" s="81"/>
-      <c r="H75" s="81"/>
-      <c r="I75" s="81"/>
-      <c r="J75" s="81"/>
-      <c r="K75" s="82"/>
-      <c r="L75" s="82"/>
-      <c r="M75" s="81"/>
-      <c r="N75" s="81"/>
+      <c r="B75" s="91"/>
+      <c r="C75" s="91"/>
+      <c r="D75" s="91"/>
+      <c r="E75" s="91"/>
+      <c r="F75" s="91"/>
+      <c r="G75" s="91"/>
+      <c r="H75" s="91"/>
+      <c r="I75" s="91"/>
+      <c r="J75" s="91"/>
+      <c r="K75" s="92"/>
+      <c r="L75" s="92"/>
+      <c r="M75" s="91"/>
+      <c r="N75" s="91"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B76" s="81"/>
-      <c r="C76" s="81"/>
-      <c r="D76" s="81"/>
-      <c r="E76" s="81"/>
-      <c r="F76" s="81"/>
-      <c r="G76" s="81"/>
-      <c r="H76" s="81"/>
-      <c r="I76" s="81"/>
-      <c r="J76" s="81"/>
-      <c r="K76" s="83"/>
-      <c r="L76" s="83"/>
-      <c r="M76" s="81"/>
-      <c r="N76" s="81"/>
+      <c r="B76" s="91"/>
+      <c r="C76" s="91"/>
+      <c r="D76" s="91"/>
+      <c r="E76" s="91"/>
+      <c r="F76" s="91"/>
+      <c r="G76" s="91"/>
+      <c r="H76" s="91"/>
+      <c r="I76" s="91"/>
+      <c r="J76" s="91"/>
+      <c r="K76" s="93"/>
+      <c r="L76" s="93"/>
+      <c r="M76" s="91"/>
+      <c r="N76" s="91"/>
     </row>
     <row r="77" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B77" s="81"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="81"/>
-      <c r="E77" s="81"/>
-      <c r="F77" s="81"/>
-      <c r="G77" s="81"/>
-      <c r="H77" s="81"/>
-      <c r="I77" s="81"/>
-      <c r="J77" s="81"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="91"/>
+      <c r="F77" s="91"/>
+      <c r="G77" s="91"/>
+      <c r="H77" s="91"/>
+      <c r="I77" s="91"/>
+      <c r="J77" s="91"/>
       <c r="K77" s="9" t="s">
         <v>14</v>
       </c>
       <c r="L77" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="M77" s="81"/>
-      <c r="N77" s="81"/>
+      <c r="M77" s="91"/>
+      <c r="N77" s="91"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B78" s="81"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="81"/>
-      <c r="F78" s="81"/>
-      <c r="G78" s="81"/>
-      <c r="H78" s="81"/>
-      <c r="I78" s="81"/>
-      <c r="J78" s="81"/>
+      <c r="B78" s="91"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="91"/>
+      <c r="E78" s="91"/>
+      <c r="F78" s="91"/>
+      <c r="G78" s="91"/>
+      <c r="H78" s="91"/>
+      <c r="I78" s="91"/>
+      <c r="J78" s="91"/>
       <c r="K78" s="9" t="s">
         <v>74</v>
       </c>
       <c r="L78" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="M78" s="81"/>
-      <c r="N78" s="81"/>
+      <c r="M78" s="91"/>
+      <c r="N78" s="91"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
@@ -13580,7 +13579,7 @@
       <c r="F150" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="G150" s="85" t="s">
+      <c r="G150" s="88" t="s">
         <v>60</v>
       </c>
       <c r="H150" s="13" t="s">
@@ -13589,11 +13588,11 @@
       <c r="I150" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J150" s="87" t="s">
+      <c r="J150" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="K150" s="87"/>
-      <c r="L150" s="85" t="s">
+      <c r="K150" s="90"/>
+      <c r="L150" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -13613,18 +13612,18 @@
       <c r="F151" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G151" s="86"/>
+      <c r="G151" s="89"/>
       <c r="H151" s="9" t="s">
         <v>119</v>
       </c>
       <c r="I151" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J151" s="84" t="s">
+      <c r="J151" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="K151" s="84"/>
-      <c r="L151" s="86"/>
+      <c r="K151" s="87"/>
+      <c r="L151" s="89"/>
     </row>
     <row r="152" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B152" s="9" t="s">
@@ -13636,18 +13635,18 @@
       <c r="F152" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G152" s="86"/>
+      <c r="G152" s="89"/>
       <c r="H152" s="9" t="s">
         <v>120</v>
       </c>
       <c r="I152" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J152" s="84" t="s">
+      <c r="J152" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K152" s="84"/>
-      <c r="L152" s="86"/>
+      <c r="K152" s="87"/>
+      <c r="L152" s="89"/>
     </row>
     <row r="153" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B153" s="9"/>
@@ -13655,18 +13654,18 @@
       <c r="D153" s="9"/>
       <c r="E153" s="9"/>
       <c r="F153" s="9"/>
-      <c r="G153" s="86"/>
+      <c r="G153" s="89"/>
       <c r="H153" s="9" t="s">
         <v>121</v>
       </c>
       <c r="I153" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J153" s="84" t="s">
+      <c r="J153" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="K153" s="84"/>
-      <c r="L153" s="86"/>
+      <c r="K153" s="87"/>
+      <c r="L153" s="89"/>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B154" s="9"/>
@@ -13674,14 +13673,14 @@
       <c r="D154" s="9"/>
       <c r="E154" s="9"/>
       <c r="F154" s="9"/>
-      <c r="G154" s="86"/>
+      <c r="G154" s="89"/>
       <c r="H154" s="9"/>
       <c r="I154" s="9"/>
-      <c r="J154" s="84" t="s">
+      <c r="J154" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="K154" s="84"/>
-      <c r="L154" s="86"/>
+      <c r="K154" s="87"/>
+      <c r="L154" s="89"/>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B155" s="9"/>
@@ -13689,14 +13688,14 @@
       <c r="D155" s="9"/>
       <c r="E155" s="9"/>
       <c r="F155" s="9"/>
-      <c r="G155" s="86"/>
+      <c r="G155" s="89"/>
       <c r="H155" s="9"/>
       <c r="I155" s="9"/>
-      <c r="J155" s="84" t="s">
+      <c r="J155" s="87" t="s">
         <v>275</v>
       </c>
-      <c r="K155" s="84"/>
-      <c r="L155" s="86"/>
+      <c r="K155" s="87"/>
+      <c r="L155" s="89"/>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B156" s="9"/>
@@ -13704,14 +13703,14 @@
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
       <c r="F156" s="9"/>
-      <c r="G156" s="86"/>
+      <c r="G156" s="89"/>
       <c r="H156" s="9"/>
       <c r="I156" s="9"/>
-      <c r="J156" s="84" t="s">
+      <c r="J156" s="87" t="s">
         <v>132</v>
       </c>
-      <c r="K156" s="84"/>
-      <c r="L156" s="86"/>
+      <c r="K156" s="87"/>
+      <c r="L156" s="89"/>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B157" s="9"/>
@@ -13719,14 +13718,14 @@
       <c r="D157" s="9"/>
       <c r="E157" s="9"/>
       <c r="F157" s="9"/>
-      <c r="G157" s="86"/>
+      <c r="G157" s="89"/>
       <c r="H157" s="9"/>
       <c r="I157" s="9"/>
-      <c r="J157" s="84" t="s">
+      <c r="J157" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="K157" s="84"/>
-      <c r="L157" s="86"/>
+      <c r="K157" s="87"/>
+      <c r="L157" s="89"/>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B158" s="9"/>
@@ -13734,14 +13733,14 @@
       <c r="D158" s="9"/>
       <c r="E158" s="9"/>
       <c r="F158" s="9"/>
-      <c r="G158" s="86"/>
+      <c r="G158" s="89"/>
       <c r="H158" s="9"/>
       <c r="I158" s="9"/>
-      <c r="J158" s="84" t="s">
+      <c r="J158" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="K158" s="84"/>
-      <c r="L158" s="86"/>
+      <c r="K158" s="87"/>
+      <c r="L158" s="89"/>
     </row>
     <row r="159" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9"/>
@@ -13749,74 +13748,74 @@
       <c r="D159" s="9"/>
       <c r="E159" s="9"/>
       <c r="F159" s="9"/>
-      <c r="G159" s="86"/>
+      <c r="G159" s="89"/>
       <c r="H159" s="9"/>
       <c r="I159" s="9"/>
-      <c r="J159" s="84" t="s">
+      <c r="J159" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="K159" s="84"/>
-      <c r="L159" s="86"/>
+      <c r="K159" s="87"/>
+      <c r="L159" s="89"/>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B160" s="81"/>
-      <c r="C160" s="81"/>
-      <c r="D160" s="81"/>
-      <c r="E160" s="81"/>
-      <c r="F160" s="81"/>
-      <c r="G160" s="81"/>
-      <c r="H160" s="81"/>
-      <c r="I160" s="81"/>
-      <c r="J160" s="82"/>
-      <c r="K160" s="82"/>
-      <c r="L160" s="81"/>
+      <c r="B160" s="91"/>
+      <c r="C160" s="91"/>
+      <c r="D160" s="91"/>
+      <c r="E160" s="91"/>
+      <c r="F160" s="91"/>
+      <c r="G160" s="91"/>
+      <c r="H160" s="91"/>
+      <c r="I160" s="91"/>
+      <c r="J160" s="92"/>
+      <c r="K160" s="92"/>
+      <c r="L160" s="91"/>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B161" s="81"/>
-      <c r="C161" s="81"/>
-      <c r="D161" s="81"/>
-      <c r="E161" s="81"/>
-      <c r="F161" s="81"/>
-      <c r="G161" s="81"/>
-      <c r="H161" s="81"/>
-      <c r="I161" s="81"/>
-      <c r="J161" s="83"/>
-      <c r="K161" s="83"/>
-      <c r="L161" s="81"/>
+      <c r="B161" s="91"/>
+      <c r="C161" s="91"/>
+      <c r="D161" s="91"/>
+      <c r="E161" s="91"/>
+      <c r="F161" s="91"/>
+      <c r="G161" s="91"/>
+      <c r="H161" s="91"/>
+      <c r="I161" s="91"/>
+      <c r="J161" s="93"/>
+      <c r="K161" s="93"/>
+      <c r="L161" s="91"/>
     </row>
     <row r="162" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B162" s="81"/>
-      <c r="C162" s="81"/>
-      <c r="D162" s="81"/>
-      <c r="E162" s="81"/>
-      <c r="F162" s="81"/>
-      <c r="G162" s="81"/>
-      <c r="H162" s="81"/>
-      <c r="I162" s="81"/>
+      <c r="B162" s="91"/>
+      <c r="C162" s="91"/>
+      <c r="D162" s="91"/>
+      <c r="E162" s="91"/>
+      <c r="F162" s="91"/>
+      <c r="G162" s="91"/>
+      <c r="H162" s="91"/>
+      <c r="I162" s="91"/>
       <c r="J162" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K162" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L162" s="81"/>
+      <c r="L162" s="91"/>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B163" s="81"/>
-      <c r="C163" s="81"/>
-      <c r="D163" s="81"/>
-      <c r="E163" s="81"/>
-      <c r="F163" s="81"/>
-      <c r="G163" s="81"/>
-      <c r="H163" s="81"/>
-      <c r="I163" s="81"/>
+      <c r="B163" s="91"/>
+      <c r="C163" s="91"/>
+      <c r="D163" s="91"/>
+      <c r="E163" s="91"/>
+      <c r="F163" s="91"/>
+      <c r="G163" s="91"/>
+      <c r="H163" s="91"/>
+      <c r="I163" s="91"/>
       <c r="J163" s="9" t="s">
         <v>74</v>
       </c>
       <c r="K163" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L163" s="81"/>
+      <c r="L163" s="91"/>
     </row>
     <row r="164" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B164" s="16" t="s">
@@ -14528,7 +14527,7 @@
       <c r="D185" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="E185" s="85" t="s">
+      <c r="E185" s="88" t="s">
         <v>60</v>
       </c>
       <c r="F185" s="13" t="s">
@@ -14537,20 +14536,20 @@
       <c r="G185" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H185" s="87" t="s">
+      <c r="H185" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="I185" s="87"/>
-      <c r="J185" s="87" t="s">
+      <c r="I185" s="90"/>
+      <c r="J185" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="K185" s="87"/>
-      <c r="L185" s="87" t="s">
+      <c r="K185" s="90"/>
+      <c r="L185" s="90" t="s">
         <v>328</v>
       </c>
-      <c r="M185" s="87"/>
-      <c r="N185" s="87"/>
-      <c r="O185" s="85" t="s">
+      <c r="M185" s="90"/>
+      <c r="N185" s="90"/>
+      <c r="O185" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -14564,27 +14563,27 @@
       <c r="D186" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E186" s="86"/>
+      <c r="E186" s="89"/>
       <c r="F186" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G186" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H186" s="84" t="s">
+      <c r="H186" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="I186" s="84"/>
-      <c r="J186" s="84" t="s">
+      <c r="I186" s="87"/>
+      <c r="J186" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="K186" s="84"/>
-      <c r="L186" s="84" t="s">
+      <c r="K186" s="87"/>
+      <c r="L186" s="87" t="s">
         <v>329</v>
       </c>
-      <c r="M186" s="84"/>
-      <c r="N186" s="84"/>
-      <c r="O186" s="86"/>
+      <c r="M186" s="87"/>
+      <c r="N186" s="87"/>
+      <c r="O186" s="89"/>
     </row>
     <row r="187" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="9" t="s">
@@ -14594,27 +14593,27 @@
       <c r="D187" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E187" s="86"/>
+      <c r="E187" s="89"/>
       <c r="F187" s="9" t="s">
         <v>120</v>
       </c>
       <c r="G187" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H187" s="84" t="s">
+      <c r="H187" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="I187" s="84"/>
-      <c r="J187" s="84" t="s">
+      <c r="I187" s="87"/>
+      <c r="J187" s="87" t="s">
         <v>325</v>
       </c>
-      <c r="K187" s="84"/>
-      <c r="L187" s="84" t="s">
+      <c r="K187" s="87"/>
+      <c r="L187" s="87" t="s">
         <v>330</v>
       </c>
-      <c r="M187" s="84"/>
-      <c r="N187" s="84"/>
-      <c r="O187" s="86"/>
+      <c r="M187" s="87"/>
+      <c r="N187" s="87"/>
+      <c r="O187" s="89"/>
     </row>
     <row r="188" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B188" s="9" t="s">
@@ -14624,27 +14623,27 @@
       <c r="D188" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E188" s="86"/>
+      <c r="E188" s="89"/>
       <c r="F188" s="9" t="s">
         <v>121</v>
       </c>
       <c r="G188" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H188" s="84" t="s">
+      <c r="H188" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="I188" s="84"/>
-      <c r="J188" s="84" t="s">
+      <c r="I188" s="87"/>
+      <c r="J188" s="87" t="s">
         <v>326</v>
       </c>
-      <c r="K188" s="84"/>
-      <c r="L188" s="84" t="s">
+      <c r="K188" s="87"/>
+      <c r="L188" s="87" t="s">
         <v>331</v>
       </c>
-      <c r="M188" s="84"/>
-      <c r="N188" s="84"/>
-      <c r="O188" s="86"/>
+      <c r="M188" s="87"/>
+      <c r="N188" s="87"/>
+      <c r="O188" s="89"/>
     </row>
     <row r="189" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="9" t="s">
@@ -14652,167 +14651,167 @@
       </c>
       <c r="C189" s="9"/>
       <c r="D189" s="9"/>
-      <c r="E189" s="86"/>
+      <c r="E189" s="89"/>
       <c r="F189" s="9"/>
       <c r="G189" s="9"/>
-      <c r="H189" s="84" t="s">
+      <c r="H189" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="I189" s="84"/>
-      <c r="J189" s="84" t="s">
+      <c r="I189" s="87"/>
+      <c r="J189" s="87" t="s">
         <v>327</v>
       </c>
-      <c r="K189" s="84"/>
-      <c r="L189" s="84" t="s">
+      <c r="K189" s="87"/>
+      <c r="L189" s="87" t="s">
         <v>332</v>
       </c>
-      <c r="M189" s="84"/>
-      <c r="N189" s="84"/>
-      <c r="O189" s="86"/>
+      <c r="M189" s="87"/>
+      <c r="N189" s="87"/>
+      <c r="O189" s="89"/>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="9"/>
-      <c r="E190" s="86"/>
+      <c r="E190" s="89"/>
       <c r="F190" s="9"/>
       <c r="G190" s="9"/>
-      <c r="H190" s="84" t="s">
+      <c r="H190" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="I190" s="84"/>
-      <c r="J190" s="84" t="s">
+      <c r="I190" s="87"/>
+      <c r="J190" s="87" t="s">
         <v>324</v>
       </c>
-      <c r="K190" s="84"/>
-      <c r="L190" s="84" t="s">
+      <c r="K190" s="87"/>
+      <c r="L190" s="87" t="s">
         <v>333</v>
       </c>
-      <c r="M190" s="84"/>
-      <c r="N190" s="84"/>
-      <c r="O190" s="86"/>
+      <c r="M190" s="87"/>
+      <c r="N190" s="87"/>
+      <c r="O190" s="89"/>
     </row>
     <row r="191" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="9"/>
-      <c r="E191" s="86"/>
+      <c r="E191" s="89"/>
       <c r="F191" s="9"/>
       <c r="G191" s="9"/>
-      <c r="H191" s="84" t="s">
+      <c r="H191" s="87" t="s">
         <v>324</v>
       </c>
-      <c r="I191" s="84"/>
-      <c r="J191" s="84" t="s">
+      <c r="I191" s="87"/>
+      <c r="J191" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="K191" s="84"/>
-      <c r="L191" s="84" t="s">
+      <c r="K191" s="87"/>
+      <c r="L191" s="87" t="s">
         <v>334</v>
       </c>
-      <c r="M191" s="84"/>
-      <c r="N191" s="84"/>
-      <c r="O191" s="86"/>
+      <c r="M191" s="87"/>
+      <c r="N191" s="87"/>
+      <c r="O191" s="89"/>
     </row>
     <row r="192" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="9"/>
-      <c r="E192" s="86"/>
+      <c r="E192" s="89"/>
       <c r="F192" s="9"/>
       <c r="G192" s="9"/>
-      <c r="H192" s="84" t="s">
+      <c r="H192" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="I192" s="84"/>
-      <c r="J192" s="84" t="s">
+      <c r="I192" s="87"/>
+      <c r="J192" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="K192" s="84"/>
-      <c r="L192" s="84" t="s">
+      <c r="K192" s="87"/>
+      <c r="L192" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="M192" s="84"/>
-      <c r="N192" s="84"/>
-      <c r="O192" s="86"/>
+      <c r="M192" s="87"/>
+      <c r="N192" s="87"/>
+      <c r="O192" s="89"/>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="9"/>
-      <c r="E193" s="86"/>
+      <c r="E193" s="89"/>
       <c r="F193" s="9"/>
       <c r="G193" s="9"/>
-      <c r="H193" s="84" t="s">
+      <c r="H193" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="I193" s="84"/>
-      <c r="J193" s="84"/>
-      <c r="K193" s="84"/>
-      <c r="L193" s="84" t="s">
+      <c r="I193" s="87"/>
+      <c r="J193" s="87"/>
+      <c r="K193" s="87"/>
+      <c r="L193" s="87" t="s">
         <v>335</v>
       </c>
-      <c r="M193" s="84"/>
-      <c r="N193" s="84"/>
-      <c r="O193" s="86"/>
+      <c r="M193" s="87"/>
+      <c r="N193" s="87"/>
+      <c r="O193" s="89"/>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
-      <c r="E194" s="86"/>
+      <c r="E194" s="89"/>
       <c r="F194" s="9"/>
       <c r="G194" s="9"/>
-      <c r="H194" s="84"/>
-      <c r="I194" s="84"/>
-      <c r="J194" s="84"/>
-      <c r="K194" s="84"/>
-      <c r="L194" s="84" t="s">
+      <c r="H194" s="87"/>
+      <c r="I194" s="87"/>
+      <c r="J194" s="87"/>
+      <c r="K194" s="87"/>
+      <c r="L194" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="M194" s="84"/>
-      <c r="N194" s="84"/>
-      <c r="O194" s="86"/>
+      <c r="M194" s="87"/>
+      <c r="N194" s="87"/>
+      <c r="O194" s="89"/>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B195" s="81"/>
-      <c r="C195" s="81"/>
-      <c r="D195" s="81"/>
-      <c r="E195" s="81"/>
-      <c r="F195" s="81"/>
-      <c r="G195" s="81"/>
-      <c r="H195" s="82"/>
-      <c r="I195" s="82"/>
-      <c r="J195" s="82"/>
-      <c r="K195" s="82"/>
-      <c r="L195" s="82"/>
-      <c r="M195" s="82"/>
-      <c r="N195" s="82"/>
-      <c r="O195" s="81"/>
+      <c r="B195" s="91"/>
+      <c r="C195" s="91"/>
+      <c r="D195" s="91"/>
+      <c r="E195" s="91"/>
+      <c r="F195" s="91"/>
+      <c r="G195" s="91"/>
+      <c r="H195" s="92"/>
+      <c r="I195" s="92"/>
+      <c r="J195" s="92"/>
+      <c r="K195" s="92"/>
+      <c r="L195" s="92"/>
+      <c r="M195" s="92"/>
+      <c r="N195" s="92"/>
+      <c r="O195" s="91"/>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B196" s="81"/>
-      <c r="C196" s="81"/>
-      <c r="D196" s="81"/>
-      <c r="E196" s="81"/>
-      <c r="F196" s="81"/>
-      <c r="G196" s="81"/>
-      <c r="H196" s="83"/>
-      <c r="I196" s="83"/>
-      <c r="J196" s="83"/>
-      <c r="K196" s="83"/>
-      <c r="L196" s="83"/>
-      <c r="M196" s="83"/>
-      <c r="N196" s="83"/>
-      <c r="O196" s="81"/>
+      <c r="B196" s="91"/>
+      <c r="C196" s="91"/>
+      <c r="D196" s="91"/>
+      <c r="E196" s="91"/>
+      <c r="F196" s="91"/>
+      <c r="G196" s="91"/>
+      <c r="H196" s="93"/>
+      <c r="I196" s="93"/>
+      <c r="J196" s="93"/>
+      <c r="K196" s="93"/>
+      <c r="L196" s="93"/>
+      <c r="M196" s="93"/>
+      <c r="N196" s="93"/>
+      <c r="O196" s="91"/>
     </row>
     <row r="197" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.3">
-      <c r="B197" s="81"/>
-      <c r="C197" s="81"/>
-      <c r="D197" s="81"/>
-      <c r="E197" s="81"/>
-      <c r="F197" s="81"/>
-      <c r="G197" s="81"/>
+      <c r="B197" s="91"/>
+      <c r="C197" s="91"/>
+      <c r="D197" s="91"/>
+      <c r="E197" s="91"/>
+      <c r="F197" s="91"/>
+      <c r="G197" s="91"/>
       <c r="H197" s="9" t="s">
         <v>14</v>
       </c>
@@ -14825,22 +14824,22 @@
       <c r="K197" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L197" s="84" t="s">
+      <c r="L197" s="87" t="s">
         <v>336</v>
       </c>
-      <c r="M197" s="84"/>
+      <c r="M197" s="87"/>
       <c r="N197" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="O197" s="81"/>
+      <c r="O197" s="91"/>
     </row>
     <row r="198" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B198" s="81"/>
-      <c r="C198" s="81"/>
-      <c r="D198" s="81"/>
-      <c r="E198" s="81"/>
-      <c r="F198" s="81"/>
-      <c r="G198" s="81"/>
+      <c r="B198" s="91"/>
+      <c r="C198" s="91"/>
+      <c r="D198" s="91"/>
+      <c r="E198" s="91"/>
+      <c r="F198" s="91"/>
+      <c r="G198" s="91"/>
       <c r="H198" s="9" t="s">
         <v>74</v>
       </c>
@@ -14853,96 +14852,96 @@
       <c r="K198" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L198" s="84" t="s">
+      <c r="L198" s="87" t="s">
         <v>337</v>
       </c>
-      <c r="M198" s="84"/>
+      <c r="M198" s="87"/>
       <c r="N198" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="O198" s="81"/>
+      <c r="O198" s="91"/>
     </row>
     <row r="199" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B199" s="81"/>
-      <c r="C199" s="81"/>
-      <c r="D199" s="81"/>
-      <c r="E199" s="81"/>
-      <c r="F199" s="81"/>
-      <c r="G199" s="81"/>
+      <c r="B199" s="91"/>
+      <c r="C199" s="91"/>
+      <c r="D199" s="91"/>
+      <c r="E199" s="91"/>
+      <c r="F199" s="91"/>
+      <c r="G199" s="91"/>
       <c r="H199" s="9"/>
       <c r="I199" s="9"/>
       <c r="J199" s="9"/>
       <c r="K199" s="9"/>
-      <c r="L199" s="84" t="s">
+      <c r="L199" s="87" t="s">
         <v>338</v>
       </c>
-      <c r="M199" s="84"/>
+      <c r="M199" s="87"/>
       <c r="N199" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="O199" s="81"/>
+      <c r="O199" s="91"/>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B200" s="81"/>
-      <c r="C200" s="81"/>
-      <c r="D200" s="81"/>
-      <c r="E200" s="81"/>
-      <c r="F200" s="81"/>
-      <c r="G200" s="81"/>
+      <c r="B200" s="91"/>
+      <c r="C200" s="91"/>
+      <c r="D200" s="91"/>
+      <c r="E200" s="91"/>
+      <c r="F200" s="91"/>
+      <c r="G200" s="91"/>
       <c r="H200" s="9"/>
       <c r="I200" s="9"/>
       <c r="J200" s="9"/>
       <c r="K200" s="9"/>
-      <c r="L200" s="84" t="s">
+      <c r="L200" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="M200" s="84"/>
+      <c r="M200" s="87"/>
       <c r="N200" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="O200" s="81"/>
+      <c r="O200" s="91"/>
     </row>
     <row r="201" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B201" s="81"/>
-      <c r="C201" s="81"/>
-      <c r="D201" s="81"/>
-      <c r="E201" s="81"/>
-      <c r="F201" s="81"/>
-      <c r="G201" s="81"/>
+      <c r="B201" s="91"/>
+      <c r="C201" s="91"/>
+      <c r="D201" s="91"/>
+      <c r="E201" s="91"/>
+      <c r="F201" s="91"/>
+      <c r="G201" s="91"/>
       <c r="H201" s="9"/>
       <c r="I201" s="9"/>
       <c r="J201" s="9"/>
       <c r="K201" s="9"/>
-      <c r="L201" s="82"/>
-      <c r="M201" s="82"/>
+      <c r="L201" s="92"/>
+      <c r="M201" s="92"/>
       <c r="N201" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="O201" s="81"/>
+      <c r="O201" s="91"/>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B202" s="81"/>
-      <c r="C202" s="81"/>
-      <c r="D202" s="81"/>
-      <c r="E202" s="81"/>
-      <c r="F202" s="81"/>
-      <c r="G202" s="81"/>
+      <c r="B202" s="91"/>
+      <c r="C202" s="91"/>
+      <c r="D202" s="91"/>
+      <c r="E202" s="91"/>
+      <c r="F202" s="91"/>
+      <c r="G202" s="91"/>
       <c r="H202" s="9"/>
       <c r="I202" s="9"/>
       <c r="J202" s="9"/>
       <c r="K202" s="9"/>
-      <c r="L202" s="83"/>
-      <c r="M202" s="83"/>
+      <c r="L202" s="93"/>
+      <c r="M202" s="93"/>
       <c r="N202" s="9"/>
-      <c r="O202" s="81"/>
+      <c r="O202" s="91"/>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B203" s="81"/>
-      <c r="C203" s="81"/>
-      <c r="D203" s="81"/>
-      <c r="E203" s="81"/>
-      <c r="F203" s="81"/>
-      <c r="G203" s="81"/>
+      <c r="B203" s="91"/>
+      <c r="C203" s="91"/>
+      <c r="D203" s="91"/>
+      <c r="E203" s="91"/>
+      <c r="F203" s="91"/>
+      <c r="G203" s="91"/>
       <c r="H203" s="9"/>
       <c r="I203" s="9"/>
       <c r="J203" s="9"/>
@@ -14954,15 +14953,15 @@
         <v>344</v>
       </c>
       <c r="N203" s="9"/>
-      <c r="O203" s="81"/>
+      <c r="O203" s="91"/>
     </row>
     <row r="204" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B204" s="81"/>
-      <c r="C204" s="81"/>
-      <c r="D204" s="81"/>
-      <c r="E204" s="81"/>
-      <c r="F204" s="81"/>
-      <c r="G204" s="81"/>
+      <c r="B204" s="91"/>
+      <c r="C204" s="91"/>
+      <c r="D204" s="91"/>
+      <c r="E204" s="91"/>
+      <c r="F204" s="91"/>
+      <c r="G204" s="91"/>
       <c r="H204" s="9"/>
       <c r="I204" s="9"/>
       <c r="J204" s="9"/>
@@ -14974,7 +14973,7 @@
         <v>59</v>
       </c>
       <c r="N204" s="9"/>
-      <c r="O204" s="81"/>
+      <c r="O204" s="91"/>
     </row>
     <row r="205" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
@@ -15636,10 +15635,10 @@
     </row>
     <row r="219" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="220" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B220" s="85" t="s">
+      <c r="B220" s="88" t="s">
         <v>407</v>
       </c>
-      <c r="C220" s="85" t="s">
+      <c r="C220" s="88" t="s">
         <v>408</v>
       </c>
       <c r="D220" s="13" t="s">
@@ -15648,202 +15647,202 @@
       <c r="E220" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="F220" s="85" t="s">
+      <c r="F220" s="88" t="s">
         <v>60</v>
       </c>
       <c r="G220" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H220" s="87" t="s">
+      <c r="H220" s="90" t="s">
         <v>412</v>
       </c>
-      <c r="I220" s="87"/>
-      <c r="J220" s="87"/>
-      <c r="K220" s="87"/>
-      <c r="L220" s="85" t="s">
+      <c r="I220" s="90"/>
+      <c r="J220" s="90"/>
+      <c r="K220" s="90"/>
+      <c r="L220" s="88" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="221" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B221" s="86"/>
-      <c r="C221" s="86"/>
+      <c r="B221" s="89"/>
+      <c r="C221" s="89"/>
       <c r="D221" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E221" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="F221" s="86"/>
+      <c r="F221" s="89"/>
       <c r="G221" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H221" s="84" t="s">
+      <c r="H221" s="87" t="s">
         <v>413</v>
       </c>
-      <c r="I221" s="84"/>
-      <c r="J221" s="84"/>
-      <c r="K221" s="84"/>
-      <c r="L221" s="86"/>
+      <c r="I221" s="87"/>
+      <c r="J221" s="87"/>
+      <c r="K221" s="87"/>
+      <c r="L221" s="89"/>
     </row>
     <row r="222" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B222" s="86"/>
-      <c r="C222" s="86"/>
+      <c r="B222" s="89"/>
+      <c r="C222" s="89"/>
       <c r="D222" s="9"/>
       <c r="E222" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="F222" s="86"/>
+      <c r="F222" s="89"/>
       <c r="G222" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H222" s="84" t="s">
+      <c r="H222" s="87" t="s">
         <v>414</v>
       </c>
-      <c r="I222" s="84"/>
-      <c r="J222" s="84"/>
-      <c r="K222" s="84"/>
-      <c r="L222" s="86"/>
+      <c r="I222" s="87"/>
+      <c r="J222" s="87"/>
+      <c r="K222" s="87"/>
+      <c r="L222" s="89"/>
     </row>
     <row r="223" spans="1:15" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B223" s="86"/>
-      <c r="C223" s="86"/>
+      <c r="B223" s="89"/>
+      <c r="C223" s="89"/>
       <c r="D223" s="9"/>
       <c r="E223" s="9"/>
-      <c r="F223" s="86"/>
+      <c r="F223" s="89"/>
       <c r="G223" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H223" s="84" t="s">
+      <c r="H223" s="87" t="s">
         <v>415</v>
       </c>
-      <c r="I223" s="84"/>
-      <c r="J223" s="84"/>
-      <c r="K223" s="84"/>
-      <c r="L223" s="86"/>
+      <c r="I223" s="87"/>
+      <c r="J223" s="87"/>
+      <c r="K223" s="87"/>
+      <c r="L223" s="89"/>
     </row>
     <row r="224" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B224" s="81"/>
-      <c r="C224" s="81"/>
-      <c r="D224" s="81"/>
-      <c r="E224" s="81"/>
-      <c r="F224" s="81"/>
-      <c r="G224" s="81"/>
-      <c r="H224" s="82"/>
-      <c r="I224" s="82"/>
-      <c r="J224" s="82"/>
-      <c r="K224" s="82"/>
-      <c r="L224" s="81"/>
+      <c r="B224" s="91"/>
+      <c r="C224" s="91"/>
+      <c r="D224" s="91"/>
+      <c r="E224" s="91"/>
+      <c r="F224" s="91"/>
+      <c r="G224" s="91"/>
+      <c r="H224" s="92"/>
+      <c r="I224" s="92"/>
+      <c r="J224" s="92"/>
+      <c r="K224" s="92"/>
+      <c r="L224" s="91"/>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B225" s="81"/>
-      <c r="C225" s="81"/>
-      <c r="D225" s="81"/>
-      <c r="E225" s="81"/>
-      <c r="F225" s="81"/>
-      <c r="G225" s="81"/>
-      <c r="H225" s="83"/>
-      <c r="I225" s="83"/>
-      <c r="J225" s="83"/>
-      <c r="K225" s="83"/>
-      <c r="L225" s="81"/>
+      <c r="B225" s="91"/>
+      <c r="C225" s="91"/>
+      <c r="D225" s="91"/>
+      <c r="E225" s="91"/>
+      <c r="F225" s="91"/>
+      <c r="G225" s="91"/>
+      <c r="H225" s="93"/>
+      <c r="I225" s="93"/>
+      <c r="J225" s="93"/>
+      <c r="K225" s="93"/>
+      <c r="L225" s="91"/>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B226" s="81"/>
-      <c r="C226" s="81"/>
-      <c r="D226" s="81"/>
-      <c r="E226" s="81"/>
-      <c r="F226" s="81"/>
-      <c r="G226" s="81"/>
-      <c r="H226" s="84" t="s">
+      <c r="B226" s="91"/>
+      <c r="C226" s="91"/>
+      <c r="D226" s="91"/>
+      <c r="E226" s="91"/>
+      <c r="F226" s="91"/>
+      <c r="G226" s="91"/>
+      <c r="H226" s="87" t="s">
         <v>416</v>
       </c>
-      <c r="I226" s="84"/>
-      <c r="J226" s="84" t="s">
+      <c r="I226" s="87"/>
+      <c r="J226" s="87" t="s">
         <v>339</v>
       </c>
-      <c r="K226" s="84"/>
-      <c r="L226" s="81"/>
+      <c r="K226" s="87"/>
+      <c r="L226" s="91"/>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B227" s="81"/>
-      <c r="C227" s="81"/>
-      <c r="D227" s="81"/>
-      <c r="E227" s="81"/>
-      <c r="F227" s="81"/>
-      <c r="G227" s="81"/>
-      <c r="H227" s="84" t="s">
+      <c r="B227" s="91"/>
+      <c r="C227" s="91"/>
+      <c r="D227" s="91"/>
+      <c r="E227" s="91"/>
+      <c r="F227" s="91"/>
+      <c r="G227" s="91"/>
+      <c r="H227" s="87" t="s">
         <v>417</v>
       </c>
-      <c r="I227" s="84"/>
-      <c r="J227" s="84" t="s">
+      <c r="I227" s="87"/>
+      <c r="J227" s="87" t="s">
         <v>418</v>
       </c>
-      <c r="K227" s="84"/>
-      <c r="L227" s="81"/>
+      <c r="K227" s="87"/>
+      <c r="L227" s="91"/>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B228" s="81"/>
-      <c r="C228" s="81"/>
-      <c r="D228" s="81"/>
-      <c r="E228" s="81"/>
-      <c r="F228" s="81"/>
-      <c r="G228" s="81"/>
-      <c r="H228" s="84"/>
-      <c r="I228" s="84"/>
-      <c r="J228" s="84" t="s">
+      <c r="B228" s="91"/>
+      <c r="C228" s="91"/>
+      <c r="D228" s="91"/>
+      <c r="E228" s="91"/>
+      <c r="F228" s="91"/>
+      <c r="G228" s="91"/>
+      <c r="H228" s="87"/>
+      <c r="I228" s="87"/>
+      <c r="J228" s="87" t="s">
         <v>419</v>
       </c>
-      <c r="K228" s="84"/>
-      <c r="L228" s="81"/>
+      <c r="K228" s="87"/>
+      <c r="L228" s="91"/>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B229" s="81"/>
-      <c r="C229" s="81"/>
-      <c r="D229" s="81"/>
-      <c r="E229" s="81"/>
-      <c r="F229" s="81"/>
-      <c r="G229" s="81"/>
-      <c r="H229" s="84"/>
-      <c r="I229" s="84"/>
-      <c r="J229" s="84" t="s">
+      <c r="B229" s="91"/>
+      <c r="C229" s="91"/>
+      <c r="D229" s="91"/>
+      <c r="E229" s="91"/>
+      <c r="F229" s="91"/>
+      <c r="G229" s="91"/>
+      <c r="H229" s="87"/>
+      <c r="I229" s="87"/>
+      <c r="J229" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="K229" s="84"/>
-      <c r="L229" s="81"/>
+      <c r="K229" s="87"/>
+      <c r="L229" s="91"/>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B230" s="81"/>
-      <c r="C230" s="81"/>
-      <c r="D230" s="81"/>
-      <c r="E230" s="81"/>
-      <c r="F230" s="81"/>
-      <c r="G230" s="81"/>
-      <c r="H230" s="82"/>
-      <c r="I230" s="82"/>
-      <c r="J230" s="82"/>
-      <c r="K230" s="82"/>
-      <c r="L230" s="81"/>
+      <c r="B230" s="91"/>
+      <c r="C230" s="91"/>
+      <c r="D230" s="91"/>
+      <c r="E230" s="91"/>
+      <c r="F230" s="91"/>
+      <c r="G230" s="91"/>
+      <c r="H230" s="92"/>
+      <c r="I230" s="92"/>
+      <c r="J230" s="92"/>
+      <c r="K230" s="92"/>
+      <c r="L230" s="91"/>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B231" s="81"/>
-      <c r="C231" s="81"/>
-      <c r="D231" s="81"/>
-      <c r="E231" s="81"/>
-      <c r="F231" s="81"/>
-      <c r="G231" s="81"/>
-      <c r="H231" s="83"/>
-      <c r="I231" s="83"/>
-      <c r="J231" s="83"/>
-      <c r="K231" s="83"/>
-      <c r="L231" s="81"/>
+      <c r="B231" s="91"/>
+      <c r="C231" s="91"/>
+      <c r="D231" s="91"/>
+      <c r="E231" s="91"/>
+      <c r="F231" s="91"/>
+      <c r="G231" s="91"/>
+      <c r="H231" s="93"/>
+      <c r="I231" s="93"/>
+      <c r="J231" s="93"/>
+      <c r="K231" s="93"/>
+      <c r="L231" s="91"/>
     </row>
     <row r="232" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B232" s="81"/>
-      <c r="C232" s="81"/>
-      <c r="D232" s="81"/>
-      <c r="E232" s="81"/>
-      <c r="F232" s="81"/>
-      <c r="G232" s="81"/>
+      <c r="B232" s="91"/>
+      <c r="C232" s="91"/>
+      <c r="D232" s="91"/>
+      <c r="E232" s="91"/>
+      <c r="F232" s="91"/>
+      <c r="G232" s="91"/>
       <c r="H232" s="9" t="s">
         <v>343</v>
       </c>
@@ -15856,15 +15855,15 @@
       <c r="K232" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="L232" s="81"/>
+      <c r="L232" s="91"/>
     </row>
     <row r="233" spans="1:12" ht="29.4" x14ac:dyDescent="0.3">
-      <c r="B233" s="81"/>
-      <c r="C233" s="81"/>
-      <c r="D233" s="81"/>
-      <c r="E233" s="81"/>
-      <c r="F233" s="81"/>
-      <c r="G233" s="81"/>
+      <c r="B233" s="91"/>
+      <c r="C233" s="91"/>
+      <c r="D233" s="91"/>
+      <c r="E233" s="91"/>
+      <c r="F233" s="91"/>
+      <c r="G233" s="91"/>
       <c r="H233" s="9" t="s">
         <v>420</v>
       </c>
@@ -15877,15 +15876,15 @@
       <c r="K233" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="L233" s="81"/>
+      <c r="L233" s="91"/>
     </row>
     <row r="234" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B234" s="81"/>
-      <c r="C234" s="81"/>
-      <c r="D234" s="81"/>
-      <c r="E234" s="81"/>
-      <c r="F234" s="81"/>
-      <c r="G234" s="81"/>
+      <c r="B234" s="91"/>
+      <c r="C234" s="91"/>
+      <c r="D234" s="91"/>
+      <c r="E234" s="91"/>
+      <c r="F234" s="91"/>
+      <c r="G234" s="91"/>
       <c r="H234" s="9"/>
       <c r="I234" s="9"/>
       <c r="J234" s="9" t="s">
@@ -15894,7 +15893,7 @@
       <c r="K234" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="L234" s="81"/>
+      <c r="L234" s="91"/>
     </row>
     <row r="235" spans="1:12" ht="63" x14ac:dyDescent="0.3">
       <c r="B235" s="10" t="s">
@@ -16413,7 +16412,7 @@
       <c r="C251" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="D251" s="85" t="s">
+      <c r="D251" s="88" t="s">
         <v>60</v>
       </c>
       <c r="E251" s="13" t="s">
@@ -16422,18 +16421,18 @@
       <c r="F251" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G251" s="87" t="s">
+      <c r="G251" s="90" t="s">
         <v>460</v>
       </c>
-      <c r="H251" s="87"/>
-      <c r="I251" s="87" t="s">
+      <c r="H251" s="90"/>
+      <c r="I251" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="J251" s="87"/>
+      <c r="J251" s="90"/>
       <c r="K251" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L251" s="85" t="s">
+      <c r="L251" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -16444,25 +16443,25 @@
       <c r="C252" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="D252" s="86"/>
+      <c r="D252" s="89"/>
       <c r="E252" s="9" t="s">
         <v>119</v>
       </c>
       <c r="F252" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G252" s="84" t="s">
+      <c r="G252" s="87" t="s">
         <v>461</v>
       </c>
-      <c r="H252" s="84"/>
-      <c r="I252" s="84" t="s">
+      <c r="H252" s="87"/>
+      <c r="I252" s="87" t="s">
         <v>463</v>
       </c>
-      <c r="J252" s="84"/>
+      <c r="J252" s="87"/>
       <c r="K252" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="L252" s="86"/>
+      <c r="L252" s="89"/>
     </row>
     <row r="253" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B253" s="9" t="s">
@@ -16471,159 +16470,159 @@
       <c r="C253" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="D253" s="86"/>
+      <c r="D253" s="89"/>
       <c r="E253" s="9" t="s">
         <v>455</v>
       </c>
       <c r="F253" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="G253" s="84" t="s">
+      <c r="G253" s="87" t="s">
         <v>462</v>
       </c>
-      <c r="H253" s="84"/>
-      <c r="I253" s="84" t="s">
+      <c r="H253" s="87"/>
+      <c r="I253" s="87" t="s">
         <v>464</v>
       </c>
-      <c r="J253" s="84"/>
+      <c r="J253" s="87"/>
       <c r="K253" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="L253" s="86"/>
+      <c r="L253" s="89"/>
     </row>
     <row r="254" spans="1:12" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="B254" s="9"/>
       <c r="C254" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="D254" s="86"/>
+      <c r="D254" s="89"/>
       <c r="E254" s="9" t="s">
         <v>456</v>
       </c>
       <c r="F254" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="G254" s="84" t="s">
+      <c r="G254" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="H254" s="84"/>
-      <c r="I254" s="84" t="s">
+      <c r="H254" s="87"/>
+      <c r="I254" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="J254" s="84"/>
+      <c r="J254" s="87"/>
       <c r="K254" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="L254" s="86"/>
+      <c r="L254" s="89"/>
     </row>
     <row r="255" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B255" s="9"/>
       <c r="C255" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="D255" s="86"/>
+      <c r="D255" s="89"/>
       <c r="E255" s="9"/>
       <c r="F255" s="9" t="s">
         <v>459</v>
       </c>
-      <c r="G255" s="84" t="s">
+      <c r="G255" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="H255" s="84"/>
-      <c r="I255" s="84" t="s">
+      <c r="H255" s="87"/>
+      <c r="I255" s="87" t="s">
         <v>465</v>
       </c>
-      <c r="J255" s="84"/>
+      <c r="J255" s="87"/>
       <c r="K255" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="L255" s="86"/>
+      <c r="L255" s="89"/>
     </row>
     <row r="256" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B256" s="9"/>
       <c r="C256" s="9"/>
-      <c r="D256" s="86"/>
+      <c r="D256" s="89"/>
       <c r="E256" s="9"/>
       <c r="F256" s="9"/>
-      <c r="G256" s="84" t="s">
+      <c r="G256" s="87" t="s">
         <v>324</v>
       </c>
-      <c r="H256" s="84"/>
-      <c r="I256" s="84" t="s">
+      <c r="H256" s="87"/>
+      <c r="I256" s="87" t="s">
         <v>466</v>
       </c>
-      <c r="J256" s="84"/>
+      <c r="J256" s="87"/>
       <c r="K256" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="L256" s="86"/>
+      <c r="L256" s="89"/>
     </row>
     <row r="257" spans="1:12" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
-      <c r="D257" s="86"/>
+      <c r="D257" s="89"/>
       <c r="E257" s="9"/>
       <c r="F257" s="9"/>
-      <c r="G257" s="84" t="s">
+      <c r="G257" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="H257" s="84"/>
-      <c r="I257" s="84" t="s">
+      <c r="H257" s="87"/>
+      <c r="I257" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="J257" s="84"/>
+      <c r="J257" s="87"/>
       <c r="K257" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="L257" s="86"/>
+      <c r="L257" s="89"/>
     </row>
     <row r="258" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
-      <c r="D258" s="86"/>
+      <c r="D258" s="89"/>
       <c r="E258" s="9"/>
       <c r="F258" s="9"/>
-      <c r="G258" s="84"/>
-      <c r="H258" s="84"/>
-      <c r="I258" s="84" t="s">
+      <c r="G258" s="87"/>
+      <c r="H258" s="87"/>
+      <c r="I258" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="J258" s="84"/>
+      <c r="J258" s="87"/>
       <c r="K258" s="9"/>
-      <c r="L258" s="86"/>
+      <c r="L258" s="89"/>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B259" s="81"/>
-      <c r="C259" s="81"/>
-      <c r="D259" s="81"/>
-      <c r="E259" s="81"/>
-      <c r="F259" s="81"/>
-      <c r="G259" s="82"/>
-      <c r="H259" s="82"/>
-      <c r="I259" s="82"/>
-      <c r="J259" s="82"/>
-      <c r="K259" s="81"/>
-      <c r="L259" s="81"/>
+      <c r="B259" s="91"/>
+      <c r="C259" s="91"/>
+      <c r="D259" s="91"/>
+      <c r="E259" s="91"/>
+      <c r="F259" s="91"/>
+      <c r="G259" s="92"/>
+      <c r="H259" s="92"/>
+      <c r="I259" s="92"/>
+      <c r="J259" s="92"/>
+      <c r="K259" s="91"/>
+      <c r="L259" s="91"/>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B260" s="81"/>
-      <c r="C260" s="81"/>
-      <c r="D260" s="81"/>
-      <c r="E260" s="81"/>
-      <c r="F260" s="81"/>
-      <c r="G260" s="83"/>
-      <c r="H260" s="83"/>
-      <c r="I260" s="83"/>
-      <c r="J260" s="83"/>
-      <c r="K260" s="81"/>
-      <c r="L260" s="81"/>
+      <c r="B260" s="91"/>
+      <c r="C260" s="91"/>
+      <c r="D260" s="91"/>
+      <c r="E260" s="91"/>
+      <c r="F260" s="91"/>
+      <c r="G260" s="93"/>
+      <c r="H260" s="93"/>
+      <c r="I260" s="93"/>
+      <c r="J260" s="93"/>
+      <c r="K260" s="91"/>
+      <c r="L260" s="91"/>
     </row>
     <row r="261" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B261" s="81"/>
-      <c r="C261" s="81"/>
-      <c r="D261" s="81"/>
-      <c r="E261" s="81"/>
-      <c r="F261" s="81"/>
+      <c r="B261" s="91"/>
+      <c r="C261" s="91"/>
+      <c r="D261" s="91"/>
+      <c r="E261" s="91"/>
+      <c r="F261" s="91"/>
       <c r="G261" s="9" t="s">
         <v>73</v>
       </c>
@@ -16636,15 +16635,15 @@
       <c r="J261" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K261" s="81"/>
-      <c r="L261" s="81"/>
+      <c r="K261" s="91"/>
+      <c r="L261" s="91"/>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B262" s="81"/>
-      <c r="C262" s="81"/>
-      <c r="D262" s="81"/>
-      <c r="E262" s="81"/>
-      <c r="F262" s="81"/>
+      <c r="B262" s="91"/>
+      <c r="C262" s="91"/>
+      <c r="D262" s="91"/>
+      <c r="E262" s="91"/>
+      <c r="F262" s="91"/>
       <c r="G262" s="9" t="s">
         <v>74</v>
       </c>
@@ -16657,8 +16656,8 @@
       <c r="J262" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K262" s="81"/>
-      <c r="L262" s="81"/>
+      <c r="K262" s="91"/>
+      <c r="L262" s="91"/>
     </row>
     <row r="263" spans="1:12" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
@@ -17332,15 +17331,15 @@
       <c r="I281" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="J281" s="87" t="s">
+      <c r="J281" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="K281" s="87"/>
-      <c r="L281" s="87" t="s">
+      <c r="K281" s="90"/>
+      <c r="L281" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="M281" s="87"/>
-      <c r="N281" s="85" t="s">
+      <c r="M281" s="90"/>
+      <c r="N281" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -17369,15 +17368,15 @@
       <c r="I282" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J282" s="84" t="s">
+      <c r="J282" s="87" t="s">
         <v>463</v>
       </c>
-      <c r="K282" s="84"/>
-      <c r="L282" s="84" t="s">
+      <c r="K282" s="87"/>
+      <c r="L282" s="87" t="s">
         <v>463</v>
       </c>
-      <c r="M282" s="84"/>
-      <c r="N282" s="86"/>
+      <c r="M282" s="87"/>
+      <c r="N282" s="89"/>
     </row>
     <row r="283" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B283" s="9" t="s">
@@ -17394,15 +17393,15 @@
       <c r="I283" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J283" s="84" t="s">
+      <c r="J283" s="87" t="s">
         <v>516</v>
       </c>
-      <c r="K283" s="84"/>
-      <c r="L283" s="84" t="s">
+      <c r="K283" s="87"/>
+      <c r="L283" s="87" t="s">
         <v>516</v>
       </c>
-      <c r="M283" s="84"/>
-      <c r="N283" s="86"/>
+      <c r="M283" s="87"/>
+      <c r="N283" s="89"/>
     </row>
     <row r="284" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B284" s="9" t="s">
@@ -17417,15 +17416,15 @@
         <v>121</v>
       </c>
       <c r="I284" s="9"/>
-      <c r="J284" s="84" t="s">
+      <c r="J284" s="87" t="s">
         <v>517</v>
       </c>
-      <c r="K284" s="84"/>
-      <c r="L284" s="84" t="s">
+      <c r="K284" s="87"/>
+      <c r="L284" s="87" t="s">
         <v>521</v>
       </c>
-      <c r="M284" s="84"/>
-      <c r="N284" s="86"/>
+      <c r="M284" s="87"/>
+      <c r="N284" s="89"/>
     </row>
     <row r="285" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B285" s="9"/>
@@ -17436,15 +17435,15 @@
       <c r="G285" s="9"/>
       <c r="H285" s="9"/>
       <c r="I285" s="9"/>
-      <c r="J285" s="84" t="s">
+      <c r="J285" s="87" t="s">
         <v>518</v>
       </c>
-      <c r="K285" s="84"/>
-      <c r="L285" s="84" t="s">
+      <c r="K285" s="87"/>
+      <c r="L285" s="87" t="s">
         <v>522</v>
       </c>
-      <c r="M285" s="84"/>
-      <c r="N285" s="86"/>
+      <c r="M285" s="87"/>
+      <c r="N285" s="89"/>
     </row>
     <row r="286" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B286" s="9"/>
@@ -17455,15 +17454,15 @@
       <c r="G286" s="9"/>
       <c r="H286" s="9"/>
       <c r="I286" s="9"/>
-      <c r="J286" s="84" t="s">
+      <c r="J286" s="87" t="s">
         <v>519</v>
       </c>
-      <c r="K286" s="84"/>
-      <c r="L286" s="84" t="s">
+      <c r="K286" s="87"/>
+      <c r="L286" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="M286" s="84"/>
-      <c r="N286" s="86"/>
+      <c r="M286" s="87"/>
+      <c r="N286" s="89"/>
     </row>
     <row r="287" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B287" s="9"/>
@@ -17474,55 +17473,55 @@
       <c r="G287" s="9"/>
       <c r="H287" s="9"/>
       <c r="I287" s="9"/>
-      <c r="J287" s="84" t="s">
+      <c r="J287" s="87" t="s">
         <v>520</v>
       </c>
-      <c r="K287" s="84"/>
-      <c r="L287" s="84" t="s">
+      <c r="K287" s="87"/>
+      <c r="L287" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="M287" s="84"/>
-      <c r="N287" s="86"/>
+      <c r="M287" s="87"/>
+      <c r="N287" s="89"/>
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B288" s="81"/>
-      <c r="C288" s="81"/>
-      <c r="D288" s="81"/>
-      <c r="E288" s="81"/>
-      <c r="F288" s="81"/>
-      <c r="G288" s="81"/>
-      <c r="H288" s="81"/>
-      <c r="I288" s="81"/>
-      <c r="J288" s="82"/>
-      <c r="K288" s="82"/>
-      <c r="L288" s="82"/>
-      <c r="M288" s="82"/>
-      <c r="N288" s="81"/>
+      <c r="B288" s="91"/>
+      <c r="C288" s="91"/>
+      <c r="D288" s="91"/>
+      <c r="E288" s="91"/>
+      <c r="F288" s="91"/>
+      <c r="G288" s="91"/>
+      <c r="H288" s="91"/>
+      <c r="I288" s="91"/>
+      <c r="J288" s="92"/>
+      <c r="K288" s="92"/>
+      <c r="L288" s="92"/>
+      <c r="M288" s="92"/>
+      <c r="N288" s="91"/>
     </row>
     <row r="289" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B289" s="81"/>
-      <c r="C289" s="81"/>
-      <c r="D289" s="81"/>
-      <c r="E289" s="81"/>
-      <c r="F289" s="81"/>
-      <c r="G289" s="81"/>
-      <c r="H289" s="81"/>
-      <c r="I289" s="81"/>
-      <c r="J289" s="83"/>
-      <c r="K289" s="83"/>
-      <c r="L289" s="83"/>
-      <c r="M289" s="83"/>
-      <c r="N289" s="81"/>
+      <c r="B289" s="91"/>
+      <c r="C289" s="91"/>
+      <c r="D289" s="91"/>
+      <c r="E289" s="91"/>
+      <c r="F289" s="91"/>
+      <c r="G289" s="91"/>
+      <c r="H289" s="91"/>
+      <c r="I289" s="91"/>
+      <c r="J289" s="93"/>
+      <c r="K289" s="93"/>
+      <c r="L289" s="93"/>
+      <c r="M289" s="93"/>
+      <c r="N289" s="91"/>
     </row>
     <row r="290" spans="1:14" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B290" s="81"/>
-      <c r="C290" s="81"/>
-      <c r="D290" s="81"/>
-      <c r="E290" s="81"/>
-      <c r="F290" s="81"/>
-      <c r="G290" s="81"/>
-      <c r="H290" s="81"/>
-      <c r="I290" s="81"/>
+      <c r="B290" s="91"/>
+      <c r="C290" s="91"/>
+      <c r="D290" s="91"/>
+      <c r="E290" s="91"/>
+      <c r="F290" s="91"/>
+      <c r="G290" s="91"/>
+      <c r="H290" s="91"/>
+      <c r="I290" s="91"/>
       <c r="J290" s="9" t="s">
         <v>14</v>
       </c>
@@ -17535,17 +17534,17 @@
       <c r="M290" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="N290" s="81"/>
+      <c r="N290" s="91"/>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B291" s="81"/>
-      <c r="C291" s="81"/>
-      <c r="D291" s="81"/>
-      <c r="E291" s="81"/>
-      <c r="F291" s="81"/>
-      <c r="G291" s="81"/>
-      <c r="H291" s="81"/>
-      <c r="I291" s="81"/>
+      <c r="B291" s="91"/>
+      <c r="C291" s="91"/>
+      <c r="D291" s="91"/>
+      <c r="E291" s="91"/>
+      <c r="F291" s="91"/>
+      <c r="G291" s="91"/>
+      <c r="H291" s="91"/>
+      <c r="I291" s="91"/>
       <c r="J291" s="9" t="s">
         <v>74</v>
       </c>
@@ -17558,7 +17557,7 @@
       <c r="M291" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="N291" s="81"/>
+      <c r="N291" s="91"/>
     </row>
     <row r="292" spans="1:14" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
@@ -18803,7 +18802,7 @@
       <c r="F322" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="G322" s="85" t="s">
+      <c r="G322" s="88" t="s">
         <v>60</v>
       </c>
       <c r="H322" s="13" t="s">
@@ -18812,11 +18811,11 @@
       <c r="I322" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J322" s="87" t="s">
+      <c r="J322" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="K322" s="87"/>
-      <c r="L322" s="85" t="s">
+      <c r="K322" s="90"/>
+      <c r="L322" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -18836,18 +18835,18 @@
       <c r="F323" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G323" s="86"/>
+      <c r="G323" s="89"/>
       <c r="H323" s="9" t="s">
         <v>119</v>
       </c>
       <c r="I323" s="9" t="s">
         <v>601</v>
       </c>
-      <c r="J323" s="84" t="s">
+      <c r="J323" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="K323" s="84"/>
-      <c r="L323" s="86"/>
+      <c r="K323" s="87"/>
+      <c r="L323" s="89"/>
     </row>
     <row r="324" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B324" s="9" t="s">
@@ -18859,18 +18858,18 @@
       <c r="F324" s="9" t="s">
         <v>600</v>
       </c>
-      <c r="G324" s="86"/>
+      <c r="G324" s="89"/>
       <c r="H324" s="9" t="s">
         <v>120</v>
       </c>
       <c r="I324" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="J324" s="84" t="s">
+      <c r="J324" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K324" s="84"/>
-      <c r="L324" s="86"/>
+      <c r="K324" s="87"/>
+      <c r="L324" s="89"/>
     </row>
     <row r="325" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
       <c r="B325" s="9" t="s">
@@ -18882,18 +18881,18 @@
       <c r="F325" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G325" s="86"/>
+      <c r="G325" s="89"/>
       <c r="H325" s="9" t="s">
         <v>121</v>
       </c>
       <c r="I325" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J325" s="84" t="s">
+      <c r="J325" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="K325" s="84"/>
-      <c r="L325" s="86"/>
+      <c r="K325" s="87"/>
+      <c r="L325" s="89"/>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B326" s="9"/>
@@ -18901,14 +18900,14 @@
       <c r="D326" s="9"/>
       <c r="E326" s="9"/>
       <c r="F326" s="9"/>
-      <c r="G326" s="86"/>
+      <c r="G326" s="89"/>
       <c r="H326" s="9"/>
       <c r="I326" s="9"/>
-      <c r="J326" s="84" t="s">
+      <c r="J326" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="K326" s="84"/>
-      <c r="L326" s="86"/>
+      <c r="K326" s="87"/>
+      <c r="L326" s="89"/>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B327" s="9"/>
@@ -18916,14 +18915,14 @@
       <c r="D327" s="9"/>
       <c r="E327" s="9"/>
       <c r="F327" s="9"/>
-      <c r="G327" s="86"/>
+      <c r="G327" s="89"/>
       <c r="H327" s="9"/>
       <c r="I327" s="9"/>
-      <c r="J327" s="84" t="s">
+      <c r="J327" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="K327" s="84"/>
-      <c r="L327" s="86"/>
+      <c r="K327" s="87"/>
+      <c r="L327" s="89"/>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B328" s="9"/>
@@ -18931,14 +18930,14 @@
       <c r="D328" s="9"/>
       <c r="E328" s="9"/>
       <c r="F328" s="9"/>
-      <c r="G328" s="86"/>
+      <c r="G328" s="89"/>
       <c r="H328" s="9"/>
       <c r="I328" s="9"/>
-      <c r="J328" s="84" t="s">
+      <c r="J328" s="87" t="s">
         <v>324</v>
       </c>
-      <c r="K328" s="84"/>
-      <c r="L328" s="86"/>
+      <c r="K328" s="87"/>
+      <c r="L328" s="89"/>
     </row>
     <row r="329" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B329" s="9"/>
@@ -18946,14 +18945,14 @@
       <c r="D329" s="9"/>
       <c r="E329" s="9"/>
       <c r="F329" s="9"/>
-      <c r="G329" s="86"/>
+      <c r="G329" s="89"/>
       <c r="H329" s="9"/>
       <c r="I329" s="9"/>
-      <c r="J329" s="84" t="s">
+      <c r="J329" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="K329" s="84"/>
-      <c r="L329" s="86"/>
+      <c r="K329" s="87"/>
+      <c r="L329" s="89"/>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B330" s="9"/>
@@ -18961,74 +18960,74 @@
       <c r="D330" s="9"/>
       <c r="E330" s="9"/>
       <c r="F330" s="9"/>
-      <c r="G330" s="86"/>
+      <c r="G330" s="89"/>
       <c r="H330" s="9"/>
       <c r="I330" s="9"/>
-      <c r="J330" s="84" t="s">
+      <c r="J330" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="K330" s="84"/>
-      <c r="L330" s="86"/>
+      <c r="K330" s="87"/>
+      <c r="L330" s="89"/>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B331" s="81"/>
-      <c r="C331" s="81"/>
-      <c r="D331" s="81"/>
-      <c r="E331" s="81"/>
-      <c r="F331" s="81"/>
-      <c r="G331" s="81"/>
-      <c r="H331" s="81"/>
-      <c r="I331" s="81"/>
-      <c r="J331" s="82"/>
-      <c r="K331" s="82"/>
-      <c r="L331" s="81"/>
+      <c r="B331" s="91"/>
+      <c r="C331" s="91"/>
+      <c r="D331" s="91"/>
+      <c r="E331" s="91"/>
+      <c r="F331" s="91"/>
+      <c r="G331" s="91"/>
+      <c r="H331" s="91"/>
+      <c r="I331" s="91"/>
+      <c r="J331" s="92"/>
+      <c r="K331" s="92"/>
+      <c r="L331" s="91"/>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B332" s="81"/>
-      <c r="C332" s="81"/>
-      <c r="D332" s="81"/>
-      <c r="E332" s="81"/>
-      <c r="F332" s="81"/>
-      <c r="G332" s="81"/>
-      <c r="H332" s="81"/>
-      <c r="I332" s="81"/>
-      <c r="J332" s="83"/>
-      <c r="K332" s="83"/>
-      <c r="L332" s="81"/>
+      <c r="B332" s="91"/>
+      <c r="C332" s="91"/>
+      <c r="D332" s="91"/>
+      <c r="E332" s="91"/>
+      <c r="F332" s="91"/>
+      <c r="G332" s="91"/>
+      <c r="H332" s="91"/>
+      <c r="I332" s="91"/>
+      <c r="J332" s="93"/>
+      <c r="K332" s="93"/>
+      <c r="L332" s="91"/>
     </row>
     <row r="333" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B333" s="81"/>
-      <c r="C333" s="81"/>
-      <c r="D333" s="81"/>
-      <c r="E333" s="81"/>
-      <c r="F333" s="81"/>
-      <c r="G333" s="81"/>
-      <c r="H333" s="81"/>
-      <c r="I333" s="81"/>
+      <c r="B333" s="91"/>
+      <c r="C333" s="91"/>
+      <c r="D333" s="91"/>
+      <c r="E333" s="91"/>
+      <c r="F333" s="91"/>
+      <c r="G333" s="91"/>
+      <c r="H333" s="91"/>
+      <c r="I333" s="91"/>
       <c r="J333" s="9" t="s">
         <v>73</v>
       </c>
       <c r="K333" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L333" s="81"/>
+      <c r="L333" s="91"/>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B334" s="81"/>
-      <c r="C334" s="81"/>
-      <c r="D334" s="81"/>
-      <c r="E334" s="81"/>
-      <c r="F334" s="81"/>
-      <c r="G334" s="81"/>
-      <c r="H334" s="81"/>
-      <c r="I334" s="81"/>
+      <c r="B334" s="91"/>
+      <c r="C334" s="91"/>
+      <c r="D334" s="91"/>
+      <c r="E334" s="91"/>
+      <c r="F334" s="91"/>
+      <c r="G334" s="91"/>
+      <c r="H334" s="91"/>
+      <c r="I334" s="91"/>
       <c r="J334" s="9" t="s">
         <v>74</v>
       </c>
       <c r="K334" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L334" s="81"/>
+      <c r="L334" s="91"/>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B335" s="10" t="s">
@@ -22435,7 +22434,7 @@
       <c r="C426" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D426" s="85" t="s">
+      <c r="D426" s="88" t="s">
         <v>60</v>
       </c>
       <c r="E426" s="13" t="s">
@@ -22444,15 +22443,15 @@
       <c r="F426" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G426" s="87" t="s">
+      <c r="G426" s="90" t="s">
         <v>683</v>
       </c>
-      <c r="H426" s="87"/>
-      <c r="I426" s="87" t="s">
+      <c r="H426" s="90"/>
+      <c r="I426" s="90" t="s">
         <v>683</v>
       </c>
-      <c r="J426" s="87"/>
-      <c r="K426" s="85" t="s">
+      <c r="J426" s="90"/>
+      <c r="K426" s="88" t="s">
         <v>17</v>
       </c>
     </row>
@@ -22463,137 +22462,137 @@
       <c r="C427" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="D427" s="86"/>
+      <c r="D427" s="89"/>
       <c r="E427" s="9" t="s">
         <v>681</v>
       </c>
       <c r="F427" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G427" s="84" t="s">
+      <c r="G427" s="87" t="s">
         <v>684</v>
       </c>
-      <c r="H427" s="84"/>
-      <c r="I427" s="84" t="s">
+      <c r="H427" s="87"/>
+      <c r="I427" s="87" t="s">
         <v>686</v>
       </c>
-      <c r="J427" s="84"/>
-      <c r="K427" s="86"/>
+      <c r="J427" s="87"/>
+      <c r="K427" s="89"/>
     </row>
     <row r="428" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B428" s="9"/>
       <c r="C428" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="D428" s="86"/>
+      <c r="D428" s="89"/>
       <c r="E428" s="9" t="s">
         <v>682</v>
       </c>
       <c r="F428" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G428" s="84" t="s">
+      <c r="G428" s="87" t="s">
         <v>685</v>
       </c>
-      <c r="H428" s="84"/>
-      <c r="I428" s="84" t="s">
+      <c r="H428" s="87"/>
+      <c r="I428" s="87" t="s">
         <v>687</v>
       </c>
-      <c r="J428" s="84"/>
-      <c r="K428" s="86"/>
+      <c r="J428" s="87"/>
+      <c r="K428" s="89"/>
     </row>
     <row r="429" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B429" s="9"/>
       <c r="C429" s="9"/>
-      <c r="D429" s="86"/>
+      <c r="D429" s="89"/>
       <c r="E429" s="9"/>
       <c r="F429" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G429" s="84" t="s">
+      <c r="G429" s="87" t="s">
         <v>522</v>
       </c>
-      <c r="H429" s="84"/>
-      <c r="I429" s="84" t="s">
+      <c r="H429" s="87"/>
+      <c r="I429" s="87" t="s">
         <v>518</v>
       </c>
-      <c r="J429" s="84"/>
-      <c r="K429" s="86"/>
+      <c r="J429" s="87"/>
+      <c r="K429" s="89"/>
     </row>
     <row r="430" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B430" s="9"/>
       <c r="C430" s="9"/>
-      <c r="D430" s="86"/>
+      <c r="D430" s="89"/>
       <c r="E430" s="9"/>
       <c r="F430" s="9"/>
-      <c r="G430" s="84" t="s">
+      <c r="G430" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="H430" s="84"/>
-      <c r="I430" s="84" t="s">
+      <c r="H430" s="87"/>
+      <c r="I430" s="87" t="s">
         <v>688</v>
       </c>
-      <c r="J430" s="84"/>
-      <c r="K430" s="86"/>
+      <c r="J430" s="87"/>
+      <c r="K430" s="89"/>
     </row>
     <row r="431" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B431" s="9"/>
       <c r="C431" s="9"/>
-      <c r="D431" s="86"/>
+      <c r="D431" s="89"/>
       <c r="E431" s="9"/>
       <c r="F431" s="9"/>
-      <c r="G431" s="84" t="s">
+      <c r="G431" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="H431" s="84"/>
-      <c r="I431" s="84"/>
-      <c r="J431" s="84"/>
-      <c r="K431" s="86"/>
+      <c r="H431" s="87"/>
+      <c r="I431" s="87"/>
+      <c r="J431" s="87"/>
+      <c r="K431" s="89"/>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B432" s="9"/>
       <c r="C432" s="9"/>
-      <c r="D432" s="86"/>
+      <c r="D432" s="89"/>
       <c r="E432" s="9"/>
       <c r="F432" s="9"/>
-      <c r="G432" s="84" t="s">
+      <c r="G432" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="H432" s="84"/>
-      <c r="I432" s="84"/>
-      <c r="J432" s="84"/>
-      <c r="K432" s="86"/>
+      <c r="H432" s="87"/>
+      <c r="I432" s="87"/>
+      <c r="J432" s="87"/>
+      <c r="K432" s="89"/>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B433" s="81"/>
-      <c r="C433" s="81"/>
-      <c r="D433" s="81"/>
-      <c r="E433" s="81"/>
-      <c r="F433" s="81"/>
-      <c r="G433" s="82"/>
-      <c r="H433" s="82"/>
-      <c r="I433" s="82"/>
-      <c r="J433" s="82"/>
-      <c r="K433" s="81"/>
+      <c r="B433" s="91"/>
+      <c r="C433" s="91"/>
+      <c r="D433" s="91"/>
+      <c r="E433" s="91"/>
+      <c r="F433" s="91"/>
+      <c r="G433" s="92"/>
+      <c r="H433" s="92"/>
+      <c r="I433" s="92"/>
+      <c r="J433" s="92"/>
+      <c r="K433" s="91"/>
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B434" s="81"/>
-      <c r="C434" s="81"/>
-      <c r="D434" s="81"/>
-      <c r="E434" s="81"/>
-      <c r="F434" s="81"/>
-      <c r="G434" s="83"/>
-      <c r="H434" s="83"/>
-      <c r="I434" s="83"/>
-      <c r="J434" s="83"/>
-      <c r="K434" s="81"/>
+      <c r="B434" s="91"/>
+      <c r="C434" s="91"/>
+      <c r="D434" s="91"/>
+      <c r="E434" s="91"/>
+      <c r="F434" s="91"/>
+      <c r="G434" s="93"/>
+      <c r="H434" s="93"/>
+      <c r="I434" s="93"/>
+      <c r="J434" s="93"/>
+      <c r="K434" s="91"/>
     </row>
     <row r="435" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B435" s="81"/>
-      <c r="C435" s="81"/>
-      <c r="D435" s="81"/>
-      <c r="E435" s="81"/>
-      <c r="F435" s="81"/>
+      <c r="B435" s="91"/>
+      <c r="C435" s="91"/>
+      <c r="D435" s="91"/>
+      <c r="E435" s="91"/>
+      <c r="F435" s="91"/>
       <c r="G435" s="9" t="s">
         <v>14</v>
       </c>
@@ -22606,14 +22605,14 @@
       <c r="J435" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K435" s="81"/>
+      <c r="K435" s="91"/>
     </row>
     <row r="436" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B436" s="81"/>
-      <c r="C436" s="81"/>
-      <c r="D436" s="81"/>
-      <c r="E436" s="81"/>
-      <c r="F436" s="81"/>
+      <c r="B436" s="91"/>
+      <c r="C436" s="91"/>
+      <c r="D436" s="91"/>
+      <c r="E436" s="91"/>
+      <c r="F436" s="91"/>
       <c r="G436" s="9" t="s">
         <v>689</v>
       </c>
@@ -22626,7 +22625,7 @@
       <c r="J436" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K436" s="81"/>
+      <c r="K436" s="91"/>
     </row>
     <row r="437" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
@@ -23120,7 +23119,7 @@
     </row>
     <row r="451" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="452" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B452" s="85" t="s">
+      <c r="B452" s="88" t="s">
         <v>407</v>
       </c>
       <c r="C452" s="13" t="s">
@@ -23129,13 +23128,13 @@
       <c r="D452" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E452" s="85" t="s">
+      <c r="E452" s="88" t="s">
         <v>720</v>
       </c>
       <c r="F452" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="G452" s="85" t="s">
+      <c r="G452" s="88" t="s">
         <v>60</v>
       </c>
       <c r="H452" s="13" t="s">
@@ -23144,208 +23143,208 @@
       <c r="I452" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J452" s="87" t="s">
+      <c r="J452" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="K452" s="87"/>
-      <c r="L452" s="85" t="s">
+      <c r="K452" s="90"/>
+      <c r="L452" s="88" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="453" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B453" s="86"/>
+      <c r="B453" s="89"/>
       <c r="C453" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D453" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E453" s="86"/>
+      <c r="E453" s="89"/>
       <c r="F453" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="G453" s="86"/>
+      <c r="G453" s="89"/>
       <c r="H453" s="9" t="s">
         <v>723</v>
       </c>
       <c r="I453" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J453" s="84" t="s">
+      <c r="J453" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="K453" s="84"/>
-      <c r="L453" s="86"/>
+      <c r="K453" s="87"/>
+      <c r="L453" s="89"/>
     </row>
     <row r="454" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B454" s="86"/>
+      <c r="B454" s="89"/>
       <c r="C454" s="9" t="s">
         <v>109</v>
       </c>
       <c r="D454" s="9"/>
-      <c r="E454" s="86"/>
+      <c r="E454" s="89"/>
       <c r="F454" s="9" t="s">
         <v>721</v>
       </c>
-      <c r="G454" s="86"/>
+      <c r="G454" s="89"/>
       <c r="H454" s="9" t="s">
         <v>120</v>
       </c>
       <c r="I454" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J454" s="84" t="s">
+      <c r="J454" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K454" s="84"/>
-      <c r="L454" s="86"/>
+      <c r="K454" s="87"/>
+      <c r="L454" s="89"/>
     </row>
     <row r="455" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B455" s="86"/>
+      <c r="B455" s="89"/>
       <c r="C455" s="9"/>
       <c r="D455" s="9"/>
-      <c r="E455" s="86"/>
+      <c r="E455" s="89"/>
       <c r="F455" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G455" s="86"/>
+      <c r="G455" s="89"/>
       <c r="H455" s="9" t="s">
         <v>121</v>
       </c>
       <c r="I455" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J455" s="84" t="s">
+      <c r="J455" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="K455" s="84"/>
-      <c r="L455" s="86"/>
+      <c r="K455" s="87"/>
+      <c r="L455" s="89"/>
     </row>
     <row r="456" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B456" s="86"/>
+      <c r="B456" s="89"/>
       <c r="C456" s="9"/>
       <c r="D456" s="9"/>
-      <c r="E456" s="86"/>
+      <c r="E456" s="89"/>
       <c r="F456" s="9" t="s">
         <v>722</v>
       </c>
-      <c r="G456" s="86"/>
+      <c r="G456" s="89"/>
       <c r="H456" s="9"/>
       <c r="I456" s="9"/>
-      <c r="J456" s="84" t="s">
+      <c r="J456" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="K456" s="84"/>
-      <c r="L456" s="86"/>
+      <c r="K456" s="87"/>
+      <c r="L456" s="89"/>
     </row>
     <row r="457" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B457" s="86"/>
+      <c r="B457" s="89"/>
       <c r="C457" s="9"/>
       <c r="D457" s="9"/>
-      <c r="E457" s="86"/>
+      <c r="E457" s="89"/>
       <c r="F457" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G457" s="86"/>
+      <c r="G457" s="89"/>
       <c r="H457" s="9"/>
       <c r="I457" s="9"/>
-      <c r="J457" s="84" t="s">
+      <c r="J457" s="87" t="s">
         <v>522</v>
       </c>
-      <c r="K457" s="84"/>
-      <c r="L457" s="86"/>
+      <c r="K457" s="87"/>
+      <c r="L457" s="89"/>
     </row>
     <row r="458" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B458" s="86"/>
+      <c r="B458" s="89"/>
       <c r="C458" s="9"/>
       <c r="D458" s="9"/>
-      <c r="E458" s="86"/>
+      <c r="E458" s="89"/>
       <c r="F458" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G458" s="86"/>
+      <c r="G458" s="89"/>
       <c r="H458" s="9"/>
       <c r="I458" s="9"/>
-      <c r="J458" s="84" t="s">
+      <c r="J458" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="K458" s="84"/>
-      <c r="L458" s="86"/>
+      <c r="K458" s="87"/>
+      <c r="L458" s="89"/>
     </row>
     <row r="459" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B459" s="86"/>
+      <c r="B459" s="89"/>
       <c r="C459" s="9"/>
       <c r="D459" s="9"/>
-      <c r="E459" s="86"/>
+      <c r="E459" s="89"/>
       <c r="F459" s="9"/>
-      <c r="G459" s="86"/>
+      <c r="G459" s="89"/>
       <c r="H459" s="9"/>
       <c r="I459" s="9"/>
-      <c r="J459" s="84" t="s">
+      <c r="J459" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="K459" s="84"/>
-      <c r="L459" s="86"/>
+      <c r="K459" s="87"/>
+      <c r="L459" s="89"/>
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B460" s="81"/>
-      <c r="C460" s="81"/>
-      <c r="D460" s="81"/>
-      <c r="E460" s="81"/>
-      <c r="F460" s="81"/>
-      <c r="G460" s="81"/>
-      <c r="H460" s="81"/>
-      <c r="I460" s="81"/>
-      <c r="J460" s="82"/>
-      <c r="K460" s="82"/>
-      <c r="L460" s="81"/>
+      <c r="B460" s="91"/>
+      <c r="C460" s="91"/>
+      <c r="D460" s="91"/>
+      <c r="E460" s="91"/>
+      <c r="F460" s="91"/>
+      <c r="G460" s="91"/>
+      <c r="H460" s="91"/>
+      <c r="I460" s="91"/>
+      <c r="J460" s="92"/>
+      <c r="K460" s="92"/>
+      <c r="L460" s="91"/>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B461" s="81"/>
-      <c r="C461" s="81"/>
-      <c r="D461" s="81"/>
-      <c r="E461" s="81"/>
-      <c r="F461" s="81"/>
-      <c r="G461" s="81"/>
-      <c r="H461" s="81"/>
-      <c r="I461" s="81"/>
-      <c r="J461" s="83"/>
-      <c r="K461" s="83"/>
-      <c r="L461" s="81"/>
+      <c r="B461" s="91"/>
+      <c r="C461" s="91"/>
+      <c r="D461" s="91"/>
+      <c r="E461" s="91"/>
+      <c r="F461" s="91"/>
+      <c r="G461" s="91"/>
+      <c r="H461" s="91"/>
+      <c r="I461" s="91"/>
+      <c r="J461" s="93"/>
+      <c r="K461" s="93"/>
+      <c r="L461" s="91"/>
     </row>
     <row r="462" spans="1:12" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B462" s="81"/>
-      <c r="C462" s="81"/>
-      <c r="D462" s="81"/>
-      <c r="E462" s="81"/>
-      <c r="F462" s="81"/>
-      <c r="G462" s="81"/>
-      <c r="H462" s="81"/>
-      <c r="I462" s="81"/>
+      <c r="B462" s="91"/>
+      <c r="C462" s="91"/>
+      <c r="D462" s="91"/>
+      <c r="E462" s="91"/>
+      <c r="F462" s="91"/>
+      <c r="G462" s="91"/>
+      <c r="H462" s="91"/>
+      <c r="I462" s="91"/>
       <c r="J462" s="9" t="s">
         <v>724</v>
       </c>
       <c r="K462" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="L462" s="81"/>
+      <c r="L462" s="91"/>
     </row>
     <row r="463" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B463" s="81"/>
-      <c r="C463" s="81"/>
-      <c r="D463" s="81"/>
-      <c r="E463" s="81"/>
-      <c r="F463" s="81"/>
-      <c r="G463" s="81"/>
-      <c r="H463" s="81"/>
-      <c r="I463" s="81"/>
+      <c r="B463" s="91"/>
+      <c r="C463" s="91"/>
+      <c r="D463" s="91"/>
+      <c r="E463" s="91"/>
+      <c r="F463" s="91"/>
+      <c r="G463" s="91"/>
+      <c r="H463" s="91"/>
+      <c r="I463" s="91"/>
       <c r="J463" s="9" t="s">
         <v>74</v>
       </c>
       <c r="K463" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L463" s="81"/>
+      <c r="L463" s="91"/>
     </row>
     <row r="464" spans="1:12" ht="126" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
@@ -23767,23 +23766,334 @@
     </row>
   </sheetData>
   <mergeCells count="369">
-    <mergeCell ref="F1:F5"/>
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K1:K5"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="D44:D53"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="L462:L463"/>
+    <mergeCell ref="J460:K461"/>
+    <mergeCell ref="L460:L461"/>
+    <mergeCell ref="B462:B463"/>
+    <mergeCell ref="C462:C463"/>
+    <mergeCell ref="D462:D463"/>
+    <mergeCell ref="E462:E463"/>
+    <mergeCell ref="F462:F463"/>
+    <mergeCell ref="G462:G463"/>
+    <mergeCell ref="H462:H463"/>
+    <mergeCell ref="I462:I463"/>
+    <mergeCell ref="J459:K459"/>
+    <mergeCell ref="L452:L459"/>
+    <mergeCell ref="B460:B461"/>
+    <mergeCell ref="C460:C461"/>
+    <mergeCell ref="D460:D461"/>
+    <mergeCell ref="E460:E461"/>
+    <mergeCell ref="F460:F461"/>
+    <mergeCell ref="G460:G461"/>
+    <mergeCell ref="H460:H461"/>
+    <mergeCell ref="I460:I461"/>
+    <mergeCell ref="B452:B459"/>
+    <mergeCell ref="E452:E459"/>
+    <mergeCell ref="G452:G459"/>
+    <mergeCell ref="J452:K452"/>
+    <mergeCell ref="J453:K453"/>
+    <mergeCell ref="J454:K454"/>
+    <mergeCell ref="J455:K455"/>
+    <mergeCell ref="J456:K456"/>
+    <mergeCell ref="J457:K457"/>
+    <mergeCell ref="J458:K458"/>
+    <mergeCell ref="B435:B436"/>
+    <mergeCell ref="C435:C436"/>
+    <mergeCell ref="D435:D436"/>
+    <mergeCell ref="E435:E436"/>
+    <mergeCell ref="F435:F436"/>
+    <mergeCell ref="K435:K436"/>
+    <mergeCell ref="K426:K432"/>
+    <mergeCell ref="B433:B434"/>
+    <mergeCell ref="C433:C434"/>
+    <mergeCell ref="D433:D434"/>
+    <mergeCell ref="E433:E434"/>
+    <mergeCell ref="F433:F434"/>
+    <mergeCell ref="G433:H434"/>
+    <mergeCell ref="I433:J434"/>
+    <mergeCell ref="K433:K434"/>
+    <mergeCell ref="I427:J427"/>
+    <mergeCell ref="I428:J428"/>
+    <mergeCell ref="I429:J429"/>
+    <mergeCell ref="I430:J430"/>
+    <mergeCell ref="I431:J431"/>
+    <mergeCell ref="I432:J432"/>
+    <mergeCell ref="D426:D432"/>
+    <mergeCell ref="G426:H426"/>
+    <mergeCell ref="G427:H427"/>
+    <mergeCell ref="G428:H428"/>
+    <mergeCell ref="G429:H429"/>
+    <mergeCell ref="G430:H430"/>
+    <mergeCell ref="G431:H431"/>
+    <mergeCell ref="G432:H432"/>
+    <mergeCell ref="I426:J426"/>
+    <mergeCell ref="B333:B334"/>
+    <mergeCell ref="C333:C334"/>
+    <mergeCell ref="D333:D334"/>
+    <mergeCell ref="E333:E334"/>
+    <mergeCell ref="F333:F334"/>
+    <mergeCell ref="G333:G334"/>
+    <mergeCell ref="H333:H334"/>
+    <mergeCell ref="I333:I334"/>
+    <mergeCell ref="L333:L334"/>
+    <mergeCell ref="L322:L330"/>
+    <mergeCell ref="B331:B332"/>
+    <mergeCell ref="C331:C332"/>
+    <mergeCell ref="D331:D332"/>
+    <mergeCell ref="E331:E332"/>
+    <mergeCell ref="F331:F332"/>
+    <mergeCell ref="G331:G332"/>
+    <mergeCell ref="H331:H332"/>
+    <mergeCell ref="I331:I332"/>
+    <mergeCell ref="J331:K332"/>
+    <mergeCell ref="L331:L332"/>
+    <mergeCell ref="G322:G330"/>
+    <mergeCell ref="J322:K322"/>
+    <mergeCell ref="J323:K323"/>
+    <mergeCell ref="J324:K324"/>
+    <mergeCell ref="J325:K325"/>
+    <mergeCell ref="J326:K326"/>
+    <mergeCell ref="J327:K327"/>
+    <mergeCell ref="J328:K328"/>
+    <mergeCell ref="J329:K329"/>
+    <mergeCell ref="J330:K330"/>
+    <mergeCell ref="B290:B291"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="D290:D291"/>
+    <mergeCell ref="E290:E291"/>
+    <mergeCell ref="F290:F291"/>
+    <mergeCell ref="G290:G291"/>
+    <mergeCell ref="H290:H291"/>
+    <mergeCell ref="I290:I291"/>
+    <mergeCell ref="N290:N291"/>
+    <mergeCell ref="L287:M287"/>
+    <mergeCell ref="J281:K281"/>
+    <mergeCell ref="J282:K282"/>
+    <mergeCell ref="J283:K283"/>
+    <mergeCell ref="J284:K284"/>
+    <mergeCell ref="J285:K285"/>
+    <mergeCell ref="J286:K286"/>
+    <mergeCell ref="L288:M289"/>
+    <mergeCell ref="N288:N289"/>
+    <mergeCell ref="B261:B262"/>
+    <mergeCell ref="C261:C262"/>
+    <mergeCell ref="D261:D262"/>
+    <mergeCell ref="E261:E262"/>
+    <mergeCell ref="F261:F262"/>
+    <mergeCell ref="K261:K262"/>
+    <mergeCell ref="L261:L262"/>
+    <mergeCell ref="N281:N287"/>
+    <mergeCell ref="B288:B289"/>
+    <mergeCell ref="C288:C289"/>
+    <mergeCell ref="D288:D289"/>
+    <mergeCell ref="E288:E289"/>
+    <mergeCell ref="F288:F289"/>
+    <mergeCell ref="G288:G289"/>
+    <mergeCell ref="H288:H289"/>
+    <mergeCell ref="I288:I289"/>
+    <mergeCell ref="J288:K289"/>
+    <mergeCell ref="J287:K287"/>
+    <mergeCell ref="L281:M281"/>
+    <mergeCell ref="L282:M282"/>
+    <mergeCell ref="L283:M283"/>
+    <mergeCell ref="L284:M284"/>
+    <mergeCell ref="L285:M285"/>
+    <mergeCell ref="L286:M286"/>
+    <mergeCell ref="K259:K260"/>
+    <mergeCell ref="L259:L260"/>
+    <mergeCell ref="D251:D258"/>
+    <mergeCell ref="G251:H251"/>
+    <mergeCell ref="G252:H252"/>
+    <mergeCell ref="G253:H253"/>
+    <mergeCell ref="G254:H254"/>
+    <mergeCell ref="G255:H255"/>
+    <mergeCell ref="I257:J257"/>
+    <mergeCell ref="I258:J258"/>
+    <mergeCell ref="L251:L258"/>
+    <mergeCell ref="B259:B260"/>
+    <mergeCell ref="C259:C260"/>
+    <mergeCell ref="D259:D260"/>
+    <mergeCell ref="E259:E260"/>
+    <mergeCell ref="F259:F260"/>
+    <mergeCell ref="G259:H260"/>
+    <mergeCell ref="I259:J260"/>
+    <mergeCell ref="I251:J251"/>
+    <mergeCell ref="I252:J252"/>
+    <mergeCell ref="I253:J253"/>
+    <mergeCell ref="I254:J254"/>
+    <mergeCell ref="I255:J255"/>
+    <mergeCell ref="I256:J256"/>
+    <mergeCell ref="G258:H258"/>
+    <mergeCell ref="G256:H256"/>
+    <mergeCell ref="G257:H257"/>
+    <mergeCell ref="B232:B234"/>
+    <mergeCell ref="C232:C234"/>
+    <mergeCell ref="D232:D234"/>
+    <mergeCell ref="E232:E234"/>
+    <mergeCell ref="F232:F234"/>
+    <mergeCell ref="G232:G234"/>
+    <mergeCell ref="L230:L231"/>
+    <mergeCell ref="H228:I228"/>
+    <mergeCell ref="H229:I229"/>
+    <mergeCell ref="D226:D229"/>
+    <mergeCell ref="E226:E229"/>
+    <mergeCell ref="F226:F229"/>
+    <mergeCell ref="G226:G229"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="D230:D231"/>
+    <mergeCell ref="E230:E231"/>
+    <mergeCell ref="F230:F231"/>
+    <mergeCell ref="G230:G231"/>
+    <mergeCell ref="H230:I231"/>
+    <mergeCell ref="J230:K231"/>
+    <mergeCell ref="L200:M200"/>
+    <mergeCell ref="O197:O200"/>
+    <mergeCell ref="L201:M202"/>
+    <mergeCell ref="O201:O202"/>
+    <mergeCell ref="L232:L234"/>
+    <mergeCell ref="H224:K225"/>
+    <mergeCell ref="L224:L225"/>
+    <mergeCell ref="L226:L229"/>
+    <mergeCell ref="L198:M198"/>
+    <mergeCell ref="J226:K226"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="H226:I226"/>
+    <mergeCell ref="H227:I227"/>
+    <mergeCell ref="B224:B225"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="D224:D225"/>
+    <mergeCell ref="E224:E225"/>
+    <mergeCell ref="F224:F225"/>
+    <mergeCell ref="G224:G225"/>
+    <mergeCell ref="B226:B229"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="B230:B231"/>
+    <mergeCell ref="O195:O196"/>
+    <mergeCell ref="B195:B196"/>
+    <mergeCell ref="C195:C196"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="E195:E196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="G195:G196"/>
+    <mergeCell ref="O203:O204"/>
+    <mergeCell ref="B220:B223"/>
+    <mergeCell ref="C220:C223"/>
+    <mergeCell ref="F220:F223"/>
+    <mergeCell ref="H220:K220"/>
+    <mergeCell ref="H221:K221"/>
+    <mergeCell ref="H222:K222"/>
+    <mergeCell ref="H223:K223"/>
+    <mergeCell ref="L220:L223"/>
+    <mergeCell ref="B197:B204"/>
+    <mergeCell ref="C197:C204"/>
+    <mergeCell ref="D197:D204"/>
+    <mergeCell ref="E197:E204"/>
+    <mergeCell ref="F197:F204"/>
+    <mergeCell ref="G197:G204"/>
+    <mergeCell ref="L197:M197"/>
+    <mergeCell ref="L199:M199"/>
+    <mergeCell ref="L192:N192"/>
+    <mergeCell ref="L193:N193"/>
+    <mergeCell ref="L194:N194"/>
+    <mergeCell ref="H190:I190"/>
+    <mergeCell ref="H191:I191"/>
+    <mergeCell ref="H192:I192"/>
+    <mergeCell ref="H193:I193"/>
+    <mergeCell ref="H194:I194"/>
+    <mergeCell ref="H195:I196"/>
+    <mergeCell ref="J195:K196"/>
+    <mergeCell ref="L195:N196"/>
+    <mergeCell ref="E185:E194"/>
+    <mergeCell ref="H185:I185"/>
+    <mergeCell ref="H186:I186"/>
+    <mergeCell ref="H187:I187"/>
+    <mergeCell ref="H188:I188"/>
+    <mergeCell ref="H189:I189"/>
+    <mergeCell ref="O185:O194"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="L185:N185"/>
+    <mergeCell ref="L186:N186"/>
+    <mergeCell ref="L187:N187"/>
+    <mergeCell ref="L188:N188"/>
+    <mergeCell ref="L189:N189"/>
+    <mergeCell ref="J185:K185"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="J188:K188"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="L190:N190"/>
+    <mergeCell ref="L191:N191"/>
+    <mergeCell ref="L160:L161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="H162:H163"/>
+    <mergeCell ref="I162:I163"/>
+    <mergeCell ref="L162:L163"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="G160:G161"/>
+    <mergeCell ref="H160:H161"/>
+    <mergeCell ref="I160:I161"/>
+    <mergeCell ref="J160:K161"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="N77:N78"/>
+    <mergeCell ref="G150:G159"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="L150:L159"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="J77:J78"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="N65:N74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="N75:N76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="I75:I76"/>
+    <mergeCell ref="J75:J76"/>
+    <mergeCell ref="K75:L76"/>
+    <mergeCell ref="M75:M76"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="D56:D57"/>
@@ -23808,334 +24118,23 @@
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="H49:I49"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="N65:N74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="N75:N76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="K75:L76"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="M77:M78"/>
-    <mergeCell ref="N77:N78"/>
-    <mergeCell ref="G150:G159"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="L150:L159"/>
-    <mergeCell ref="L160:L161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="G162:G163"/>
-    <mergeCell ref="H162:H163"/>
-    <mergeCell ref="I162:I163"/>
-    <mergeCell ref="L162:L163"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="G160:G161"/>
-    <mergeCell ref="H160:H161"/>
-    <mergeCell ref="I160:I161"/>
-    <mergeCell ref="J160:K161"/>
-    <mergeCell ref="E185:E194"/>
-    <mergeCell ref="H185:I185"/>
-    <mergeCell ref="H186:I186"/>
-    <mergeCell ref="H187:I187"/>
-    <mergeCell ref="H188:I188"/>
-    <mergeCell ref="H189:I189"/>
-    <mergeCell ref="O185:O194"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="L185:N185"/>
-    <mergeCell ref="L186:N186"/>
-    <mergeCell ref="L187:N187"/>
-    <mergeCell ref="L188:N188"/>
-    <mergeCell ref="L189:N189"/>
-    <mergeCell ref="J185:K185"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="J188:K188"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="L190:N190"/>
-    <mergeCell ref="L191:N191"/>
-    <mergeCell ref="L192:N192"/>
-    <mergeCell ref="L193:N193"/>
-    <mergeCell ref="L194:N194"/>
-    <mergeCell ref="H190:I190"/>
-    <mergeCell ref="H191:I191"/>
-    <mergeCell ref="H192:I192"/>
-    <mergeCell ref="H193:I193"/>
-    <mergeCell ref="H194:I194"/>
-    <mergeCell ref="H195:I196"/>
-    <mergeCell ref="J195:K196"/>
-    <mergeCell ref="L195:N196"/>
-    <mergeCell ref="O195:O196"/>
-    <mergeCell ref="B195:B196"/>
-    <mergeCell ref="C195:C196"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="G195:G196"/>
-    <mergeCell ref="O203:O204"/>
-    <mergeCell ref="B220:B223"/>
-    <mergeCell ref="C220:C223"/>
-    <mergeCell ref="F220:F223"/>
-    <mergeCell ref="H220:K220"/>
-    <mergeCell ref="H221:K221"/>
-    <mergeCell ref="H222:K222"/>
-    <mergeCell ref="H223:K223"/>
-    <mergeCell ref="L220:L223"/>
-    <mergeCell ref="B197:B204"/>
-    <mergeCell ref="C197:C204"/>
-    <mergeCell ref="D197:D204"/>
-    <mergeCell ref="E197:E204"/>
-    <mergeCell ref="F197:F204"/>
-    <mergeCell ref="G197:G204"/>
-    <mergeCell ref="L197:M197"/>
-    <mergeCell ref="L199:M199"/>
-    <mergeCell ref="B224:B225"/>
-    <mergeCell ref="C224:C225"/>
-    <mergeCell ref="D224:D225"/>
-    <mergeCell ref="E224:E225"/>
-    <mergeCell ref="F224:F225"/>
-    <mergeCell ref="G224:G225"/>
-    <mergeCell ref="B226:B229"/>
-    <mergeCell ref="C226:C229"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="L200:M200"/>
-    <mergeCell ref="O197:O200"/>
-    <mergeCell ref="L201:M202"/>
-    <mergeCell ref="O201:O202"/>
-    <mergeCell ref="L232:L234"/>
-    <mergeCell ref="H224:K225"/>
-    <mergeCell ref="L224:L225"/>
-    <mergeCell ref="L226:L229"/>
-    <mergeCell ref="L198:M198"/>
-    <mergeCell ref="J226:K226"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="J228:K228"/>
-    <mergeCell ref="J229:K229"/>
-    <mergeCell ref="H226:I226"/>
-    <mergeCell ref="H227:I227"/>
-    <mergeCell ref="B232:B234"/>
-    <mergeCell ref="C232:C234"/>
-    <mergeCell ref="D232:D234"/>
-    <mergeCell ref="E232:E234"/>
-    <mergeCell ref="F232:F234"/>
-    <mergeCell ref="G232:G234"/>
-    <mergeCell ref="L230:L231"/>
-    <mergeCell ref="H228:I228"/>
-    <mergeCell ref="H229:I229"/>
-    <mergeCell ref="D226:D229"/>
-    <mergeCell ref="E226:E229"/>
-    <mergeCell ref="F226:F229"/>
-    <mergeCell ref="G226:G229"/>
-    <mergeCell ref="C230:C231"/>
-    <mergeCell ref="D230:D231"/>
-    <mergeCell ref="E230:E231"/>
-    <mergeCell ref="F230:F231"/>
-    <mergeCell ref="G230:G231"/>
-    <mergeCell ref="H230:I231"/>
-    <mergeCell ref="J230:K231"/>
-    <mergeCell ref="B259:B260"/>
-    <mergeCell ref="C259:C260"/>
-    <mergeCell ref="D259:D260"/>
-    <mergeCell ref="E259:E260"/>
-    <mergeCell ref="F259:F260"/>
-    <mergeCell ref="G259:H260"/>
-    <mergeCell ref="I259:J260"/>
-    <mergeCell ref="I251:J251"/>
-    <mergeCell ref="I252:J252"/>
-    <mergeCell ref="I253:J253"/>
-    <mergeCell ref="I254:J254"/>
-    <mergeCell ref="I255:J255"/>
-    <mergeCell ref="I256:J256"/>
-    <mergeCell ref="G258:H258"/>
-    <mergeCell ref="G256:H256"/>
-    <mergeCell ref="G257:H257"/>
-    <mergeCell ref="K259:K260"/>
-    <mergeCell ref="L259:L260"/>
-    <mergeCell ref="D251:D258"/>
-    <mergeCell ref="G251:H251"/>
-    <mergeCell ref="G252:H252"/>
-    <mergeCell ref="G253:H253"/>
-    <mergeCell ref="G254:H254"/>
-    <mergeCell ref="G255:H255"/>
-    <mergeCell ref="I257:J257"/>
-    <mergeCell ref="I258:J258"/>
-    <mergeCell ref="L251:L258"/>
-    <mergeCell ref="B261:B262"/>
-    <mergeCell ref="C261:C262"/>
-    <mergeCell ref="D261:D262"/>
-    <mergeCell ref="E261:E262"/>
-    <mergeCell ref="F261:F262"/>
-    <mergeCell ref="K261:K262"/>
-    <mergeCell ref="L261:L262"/>
-    <mergeCell ref="N281:N287"/>
-    <mergeCell ref="B288:B289"/>
-    <mergeCell ref="C288:C289"/>
-    <mergeCell ref="D288:D289"/>
-    <mergeCell ref="E288:E289"/>
-    <mergeCell ref="F288:F289"/>
-    <mergeCell ref="G288:G289"/>
-    <mergeCell ref="H288:H289"/>
-    <mergeCell ref="I288:I289"/>
-    <mergeCell ref="J288:K289"/>
-    <mergeCell ref="J287:K287"/>
-    <mergeCell ref="L281:M281"/>
-    <mergeCell ref="L282:M282"/>
-    <mergeCell ref="L283:M283"/>
-    <mergeCell ref="L284:M284"/>
-    <mergeCell ref="L285:M285"/>
-    <mergeCell ref="L286:M286"/>
-    <mergeCell ref="L287:M287"/>
-    <mergeCell ref="J281:K281"/>
-    <mergeCell ref="J282:K282"/>
-    <mergeCell ref="J283:K283"/>
-    <mergeCell ref="J284:K284"/>
-    <mergeCell ref="J285:K285"/>
-    <mergeCell ref="J286:K286"/>
-    <mergeCell ref="L288:M289"/>
-    <mergeCell ref="N288:N289"/>
-    <mergeCell ref="B290:B291"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="D290:D291"/>
-    <mergeCell ref="E290:E291"/>
-    <mergeCell ref="F290:F291"/>
-    <mergeCell ref="G290:G291"/>
-    <mergeCell ref="H290:H291"/>
-    <mergeCell ref="I290:I291"/>
-    <mergeCell ref="N290:N291"/>
-    <mergeCell ref="L333:L334"/>
-    <mergeCell ref="L322:L330"/>
-    <mergeCell ref="B331:B332"/>
-    <mergeCell ref="C331:C332"/>
-    <mergeCell ref="D331:D332"/>
-    <mergeCell ref="E331:E332"/>
-    <mergeCell ref="F331:F332"/>
-    <mergeCell ref="G331:G332"/>
-    <mergeCell ref="H331:H332"/>
-    <mergeCell ref="I331:I332"/>
-    <mergeCell ref="J331:K332"/>
-    <mergeCell ref="L331:L332"/>
-    <mergeCell ref="G322:G330"/>
-    <mergeCell ref="J322:K322"/>
-    <mergeCell ref="J323:K323"/>
-    <mergeCell ref="J324:K324"/>
-    <mergeCell ref="J325:K325"/>
-    <mergeCell ref="J326:K326"/>
-    <mergeCell ref="J327:K327"/>
-    <mergeCell ref="J328:K328"/>
-    <mergeCell ref="J329:K329"/>
-    <mergeCell ref="J330:K330"/>
-    <mergeCell ref="G428:H428"/>
-    <mergeCell ref="G429:H429"/>
-    <mergeCell ref="G430:H430"/>
-    <mergeCell ref="G431:H431"/>
-    <mergeCell ref="G432:H432"/>
-    <mergeCell ref="I426:J426"/>
-    <mergeCell ref="B333:B334"/>
-    <mergeCell ref="C333:C334"/>
-    <mergeCell ref="D333:D334"/>
-    <mergeCell ref="E333:E334"/>
-    <mergeCell ref="F333:F334"/>
-    <mergeCell ref="G333:G334"/>
-    <mergeCell ref="H333:H334"/>
-    <mergeCell ref="I333:I334"/>
-    <mergeCell ref="B435:B436"/>
-    <mergeCell ref="C435:C436"/>
-    <mergeCell ref="D435:D436"/>
-    <mergeCell ref="E435:E436"/>
-    <mergeCell ref="F435:F436"/>
-    <mergeCell ref="K435:K436"/>
-    <mergeCell ref="K426:K432"/>
-    <mergeCell ref="B433:B434"/>
-    <mergeCell ref="C433:C434"/>
-    <mergeCell ref="D433:D434"/>
-    <mergeCell ref="E433:E434"/>
-    <mergeCell ref="F433:F434"/>
-    <mergeCell ref="G433:H434"/>
-    <mergeCell ref="I433:J434"/>
-    <mergeCell ref="K433:K434"/>
-    <mergeCell ref="I427:J427"/>
-    <mergeCell ref="I428:J428"/>
-    <mergeCell ref="I429:J429"/>
-    <mergeCell ref="I430:J430"/>
-    <mergeCell ref="I431:J431"/>
-    <mergeCell ref="I432:J432"/>
-    <mergeCell ref="D426:D432"/>
-    <mergeCell ref="G426:H426"/>
-    <mergeCell ref="G427:H427"/>
-    <mergeCell ref="J459:K459"/>
-    <mergeCell ref="L452:L459"/>
-    <mergeCell ref="B460:B461"/>
-    <mergeCell ref="C460:C461"/>
-    <mergeCell ref="D460:D461"/>
-    <mergeCell ref="E460:E461"/>
-    <mergeCell ref="F460:F461"/>
-    <mergeCell ref="G460:G461"/>
-    <mergeCell ref="H460:H461"/>
-    <mergeCell ref="I460:I461"/>
-    <mergeCell ref="B452:B459"/>
-    <mergeCell ref="E452:E459"/>
-    <mergeCell ref="G452:G459"/>
-    <mergeCell ref="J452:K452"/>
-    <mergeCell ref="J453:K453"/>
-    <mergeCell ref="J454:K454"/>
-    <mergeCell ref="J455:K455"/>
-    <mergeCell ref="J456:K456"/>
-    <mergeCell ref="J457:K457"/>
-    <mergeCell ref="J458:K458"/>
-    <mergeCell ref="L462:L463"/>
-    <mergeCell ref="J460:K461"/>
-    <mergeCell ref="L460:L461"/>
-    <mergeCell ref="B462:B463"/>
-    <mergeCell ref="C462:C463"/>
-    <mergeCell ref="D462:D463"/>
-    <mergeCell ref="E462:E463"/>
-    <mergeCell ref="F462:F463"/>
-    <mergeCell ref="G462:G463"/>
-    <mergeCell ref="H462:H463"/>
-    <mergeCell ref="I462:I463"/>
+    <mergeCell ref="F1:F5"/>
+    <mergeCell ref="G1:G5"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K1:K5"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="D44:D53"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="TFN1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5788731/table/T1/?report=objectonly - TFN1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -35676,7 +35675,7 @@
   <dimension ref="A2:AI34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35738,7 +35737,7 @@
       </c>
       <c r="I2" s="29">
         <f ca="1">C2*_xll.PsiUniform(1-H2,1+H2)</f>
-        <v>196905.6218109022</v>
+        <v>200056.19754821275</v>
       </c>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
@@ -35799,7 +35798,7 @@
       </c>
       <c r="C6" s="38">
         <f ca="1">SUM($P$11:$P$30)</f>
-        <v>2043.655925508672</v>
+        <v>2043.7298405000004</v>
       </c>
       <c r="E6" s="29"/>
       <c r="G6" s="29"/>
@@ -35814,7 +35813,7 @@
       </c>
       <c r="C7" s="38">
         <f ca="1">$C$4-$C$6</f>
-        <v>17.344074491328001</v>
+        <v>17.270159499999636</v>
       </c>
       <c r="E7" s="29"/>
       <c r="G7" s="29"/>
@@ -35947,7 +35946,7 @@
       </c>
       <c r="C11" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I2:I10)/100</f>
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="D11" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B11,Combined!H:H)</f>
@@ -35996,7 +35995,7 @@
       </c>
       <c r="P11" s="78">
         <f t="shared" ref="P11:P29" ca="1" si="3">(N11*$C$5)*(1-C11)</f>
-        <v>5.8161490428277505E-3</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="78">
         <f t="shared" ref="Q11:Q29" si="4">R11*K11/$K$30</f>
@@ -36064,7 +36063,7 @@
       </c>
       <c r="C12" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I3:I11)/100</f>
-        <v>0.69</v>
+        <v>1</v>
       </c>
       <c r="D12" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B12,Combined!H:H)</f>
@@ -36412,7 +36411,7 @@
       </c>
       <c r="C15" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I6:I14)/100</f>
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="D15" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B15,Combined!H:H)</f>
@@ -36460,7 +36459,7 @@
       </c>
       <c r="P15" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>3.278193096866553E-3</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="78">
         <f t="shared" si="4"/>
@@ -36644,7 +36643,7 @@
       </c>
       <c r="C17" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I8:I16)/100</f>
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="D17" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B17,Combined!H:H)</f>
@@ -36693,7 +36692,7 @@
       </c>
       <c r="P17" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4171009009154307E-4</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="78">
         <f t="shared" si="4"/>
@@ -36761,7 +36760,7 @@
       </c>
       <c r="C18" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I9:I17)/100</f>
-        <v>0.95</v>
+        <v>0.45</v>
       </c>
       <c r="D18" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B18,Combined!H:H)</f>
@@ -36810,7 +36809,7 @@
       </c>
       <c r="P18" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0402597269326903E-3</v>
+        <v>3.3442856996259568E-2</v>
       </c>
       <c r="Q18" s="78">
         <f t="shared" si="4"/>
@@ -36878,7 +36877,7 @@
       </c>
       <c r="C19" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I10:I18)/100</f>
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="D19" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B19,Combined!H:H)</f>
@@ -36925,7 +36924,7 @@
       </c>
       <c r="P19" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22883902779416843</v>
+        <v>0.17162927084562632</v>
       </c>
       <c r="Q19" s="78">
         <f t="shared" si="4"/>
@@ -36993,7 +36992,7 @@
       </c>
       <c r="C20" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I11:I19)/100</f>
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="D20" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B20,Combined!H:H)</f>
@@ -37110,7 +37109,7 @@
       </c>
       <c r="C21" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I12:I20)/100</f>
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="D21" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B21,Combined!H:H)</f>
@@ -37227,7 +37226,7 @@
       </c>
       <c r="C22" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I13:I21)/100</f>
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="D22" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B22,Combined!H:H)</f>
@@ -37274,7 +37273,7 @@
       </c>
       <c r="P22" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2860487847427105</v>
+        <v>0.40046829863979411</v>
       </c>
       <c r="Q22" s="78">
         <f t="shared" si="4"/>
@@ -37342,7 +37341,7 @@
       </c>
       <c r="C23" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I14:I22)/100</f>
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="D23" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B23,Combined!H:H)</f>
@@ -37391,7 +37390,7 @@
       </c>
       <c r="P23" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7104008784127054E-3</v>
+        <v>9.5173347973545076E-3</v>
       </c>
       <c r="Q23" s="78">
         <f t="shared" si="4"/>
@@ -37459,7 +37458,7 @@
       </c>
       <c r="C24" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I15:I23)/100</f>
-        <v>0.56999999999999995</v>
+        <v>0.87</v>
       </c>
       <c r="D24" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B24,Combined!H:H)</f>
@@ -37506,7 +37505,7 @@
       </c>
       <c r="P24" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0255580220228213E-2</v>
+        <v>6.1237800665806218E-3</v>
       </c>
       <c r="Q24" s="78">
         <f t="shared" si="4"/>
@@ -37574,7 +37573,7 @@
       </c>
       <c r="C25" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I16:I24)/100</f>
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="D25" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B25,Combined!H:H)</f>
@@ -37621,7 +37620,7 @@
       </c>
       <c r="P25" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9.1648409159710009E-3</v>
       </c>
       <c r="Q25" s="78">
         <f t="shared" si="4"/>
@@ -37804,7 +37803,7 @@
       </c>
       <c r="C27" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I18:I26)/100</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="D27" s="71">
         <f>AVERAGEIF(Combined!B:B,'Model - Rough with weights (2)'!B27,Combined!H:H)</f>
@@ -37851,7 +37850,7 @@
       </c>
       <c r="P27" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>2.3553000256079336E-3</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="78">
         <f t="shared" si="4"/>
@@ -38037,7 +38036,7 @@
       </c>
       <c r="C29" s="68">
         <f ca="1">_xll.PsiDisUniform(Combined!I20:I28)/100</f>
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="D29" s="71">
         <v>26</v>
@@ -38081,7 +38080,7 @@
       </c>
       <c r="P29" s="78">
         <f t="shared" ca="1" si="3"/>
-        <v>1.057481644150501E-3</v>
+        <v>2.1149632883010018E-4</v>
       </c>
       <c r="Q29" s="78">
         <f t="shared" si="4"/>
@@ -39713,8 +39712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608B5213-9F09-43B6-9AE7-31EEFEE9D58A}">
   <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>